<commit_message>
corrected upper speaker positions
</commit_message>
<xml_diff>
--- a/speakerpositions/Hufo_allSpeakerpositions.xlsx
+++ b/speakerpositions/Hufo_allSpeakerpositions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psch/Documents/GitHub/hufo_system/speakerpositions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{852EB9E6-D745-FD4F-A384-646F5D8E05A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA3E905A-30C2-F449-84BC-95A3FA31838E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12160" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{5ABADEA7-2DF9-5341-AACA-1736DC7CEC8A}"/>
   </bookViews>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB4A2B6-EB8A-6A43-B754-121A2528DB3A}">
   <dimension ref="A2:Y89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="W87" activeCellId="2" sqref="S87 V87 W87"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="Q96" sqref="Q96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6738,18 +6738,20 @@
         <v>3062.03</v>
       </c>
       <c r="H83" s="3">
-        <v>-5283.832018150646</v>
+        <f>H79*-1</f>
+        <v>5286.3950181506461</v>
       </c>
       <c r="I83" s="3">
-        <v>2646.1271955159245</v>
+        <f>I79*-1</f>
+        <v>-2644.5681955159243</v>
       </c>
       <c r="K83" s="20">
         <f>H83/1000</f>
-        <v>-5.2838320181506457</v>
+        <v>5.2863950181506461</v>
       </c>
       <c r="L83" s="21">
         <f>I83/1000</f>
-        <v>2.6461271955159247</v>
+        <v>-2.6445681955159244</v>
       </c>
       <c r="M83" s="22">
         <f>G83/1000</f>
@@ -6766,31 +6768,31 @@
       </c>
       <c r="S83" s="20">
         <f>DEGREES( ATAN2(L83,K83))</f>
-        <v>-63.398428921421988</v>
+        <v>116.57693472378661</v>
       </c>
       <c r="T83" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K83,2)+POWER(L83,2))),M83))</f>
-        <v>27.391547369746746</v>
+        <v>27.385235002966883</v>
       </c>
       <c r="U83" s="21">
         <f>SQRT(POWER(K83,2)+POWER(L83,2)+POWER(M83,2))</f>
-        <v>6.6555914576980237</v>
+        <v>6.6570069062276271</v>
       </c>
       <c r="V83" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K83,2)+POWER(L83,2))),O83))</f>
-        <v>12.518021148079114</v>
+        <v>12.514751523165046</v>
       </c>
       <c r="W83" s="21">
         <f>SQRT(POWER(K83,2)+POWER(L83,2)+POWER(O83,2))</f>
-        <v>6.0532877555740647</v>
+        <v>6.0548440070378629</v>
       </c>
       <c r="X83" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K83,2)+POWER(L83,2))),Q83))</f>
-        <v>10.059657150098166</v>
+        <v>10.056999542825952</v>
       </c>
       <c r="Y83" s="22">
         <f>SQRT(POWER(K83,2)+POWER(L83,2)+POWER(Q83,2))</f>
-        <v>6.0016552483279897</v>
+        <v>6.0032248848066923</v>
       </c>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.2">
@@ -6819,18 +6821,20 @@
         <v>3062.03</v>
       </c>
       <c r="H84" s="3">
-        <v>-1838.7873034655597</v>
+        <f t="shared" ref="H84:I84" si="20">H80*-1</f>
+        <v>1895.5093034655597</v>
       </c>
       <c r="I84" s="3">
-        <v>4034.1932779274421</v>
+        <f t="shared" si="20"/>
+        <v>-4022.0862779274421</v>
       </c>
       <c r="K84" s="20">
         <f>H84/1000</f>
-        <v>-1.8387873034655597</v>
+        <v>1.8955093034655597</v>
       </c>
       <c r="L84" s="21">
         <f>I84/1000</f>
-        <v>4.0341932779274421</v>
+        <v>-4.0220862779274418</v>
       </c>
       <c r="M84" s="22">
         <f>G84/1000</f>
@@ -6847,31 +6851,31 @@
       </c>
       <c r="S84" s="20">
         <f>DEGREES( ATAN2(L84,K84))</f>
-        <v>-24.503522137434636</v>
+        <v>154.76666329522828</v>
       </c>
       <c r="T84" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K84,2)+POWER(L84,2))),M84))</f>
-        <v>34.631235178960253</v>
+        <v>34.553616538294953</v>
       </c>
       <c r="U84" s="21">
         <f>SQRT(POWER(K84,2)+POWER(L84,2)+POWER(M84,2))</f>
-        <v>5.3881241514984701</v>
+        <v>5.398718483817869</v>
       </c>
       <c r="V84" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K84,2)+POWER(L84,2))),O84))</f>
-        <v>16.485382316912638</v>
+        <v>16.440246799953421</v>
       </c>
       <c r="W84" s="21">
         <f>SQRT(POWER(K84,2)+POWER(L84,2)+POWER(O84,2))</f>
-        <v>4.6235567339399122</v>
+        <v>4.6358986472437804</v>
       </c>
       <c r="X84" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K84,2)+POWER(L84,2))),Q84))</f>
-        <v>13.303632931919649</v>
+        <v>13.26649045905646</v>
       </c>
       <c r="Y84" s="22">
         <f>SQRT(POWER(K84,2)+POWER(L84,2)+POWER(Q84,2))</f>
-        <v>4.5557491085397919</v>
+        <v>4.5682742185114842</v>
       </c>
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.2">
@@ -6900,18 +6904,20 @@
         <v>3062.03</v>
       </c>
       <c r="H85" s="3">
-        <v>1838.7873034655597</v>
+        <f t="shared" ref="H85:I85" si="21">H81*-1</f>
+        <v>-1861.2803034655599</v>
       </c>
       <c r="I85" s="3">
-        <v>4039.6219999999998</v>
+        <f t="shared" si="21"/>
+        <v>-4034.6122634598378</v>
       </c>
       <c r="K85" s="20">
         <f>H85/1000</f>
-        <v>1.8387873034655597</v>
+        <v>-1.8612803034655598</v>
       </c>
       <c r="L85" s="21">
         <f>I85/1000</f>
-        <v>4.0396219999999996</v>
+        <v>-4.034612263459838</v>
       </c>
       <c r="M85" s="22">
         <f>G85/1000</f>
@@ -6928,31 +6934,31 @@
       </c>
       <c r="S85" s="20">
         <f>DEGREES( ATAN2(L85,K85))</f>
-        <v>24.47445674721007</v>
+        <v>-155.23479302123613</v>
       </c>
       <c r="T85" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K85,2)+POWER(L85,2))),M85))</f>
-        <v>34.601402800999509</v>
+        <v>34.572363524646619</v>
       </c>
       <c r="U85" s="21">
         <f>SQRT(POWER(K85,2)+POWER(L85,2)+POWER(M85,2))</f>
-        <v>5.3921899420523145</v>
+        <v>5.3961549463881564</v>
       </c>
       <c r="V85" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K85,2)+POWER(L85,2))),O85))</f>
-        <v>16.468027189366833</v>
+        <v>16.451142441190825</v>
       </c>
       <c r="W85" s="21">
         <f>SQRT(POWER(K85,2)+POWER(L85,2)+POWER(O85,2))</f>
-        <v>4.628294218302262</v>
+        <v>4.6329130366789064</v>
       </c>
       <c r="X85" s="21">
         <f>DEGREES(ATAN2((SQRT(POWER(K85,2)+POWER(L85,2))),Q85))</f>
-        <v>13.289350521250501</v>
+        <v>13.275456050147248</v>
       </c>
       <c r="Y85" s="22">
         <f>SQRT(POWER(K85,2)+POWER(L85,2)+POWER(Q85,2))</f>
-        <v>4.5605570316760806</v>
+        <v>4.5652443826622653</v>
       </c>
     </row>
     <row r="86" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -6980,19 +6986,21 @@
       <c r="G86" s="4">
         <v>3062.03</v>
       </c>
-      <c r="H86" s="49">
-        <v>5292.7826070532083</v>
-      </c>
-      <c r="I86" s="49">
-        <v>2640.7024930611842</v>
+      <c r="H86" s="3">
+        <f t="shared" ref="H86:I86" si="22">H82*-1</f>
+        <v>-5306.4506070532079</v>
+      </c>
+      <c r="I86" s="3">
+        <f t="shared" si="22"/>
+        <v>-2632.384493061184</v>
       </c>
       <c r="K86" s="23">
         <f>H86/1000</f>
-        <v>5.2927826070532085</v>
+        <v>-5.3064506070532076</v>
       </c>
       <c r="L86" s="24">
         <f>I86/1000</f>
-        <v>2.6407024930611844</v>
+        <v>-2.6323844930611839</v>
       </c>
       <c r="M86" s="25">
         <f>G86/1000</f>
@@ -7009,31 +7017,31 @@
       </c>
       <c r="S86" s="23">
         <f>DEGREES( ATAN2(L86,K86))</f>
-        <v>63.484236310055316</v>
+        <v>-116.3847475481442</v>
       </c>
       <c r="T86" s="24">
         <f>DEGREES(ATAN2((SQRT(POWER(K86,2)+POWER(L86,2))),M86))</f>
-        <v>27.369461253572339</v>
+        <v>27.335757209509374</v>
       </c>
       <c r="U86" s="24">
         <f>SQRT(POWER(K86,2)+POWER(L86,2)+POWER(M86,2))</f>
-        <v>6.6605469072204961</v>
+        <v>6.6681252151788772</v>
       </c>
       <c r="V86" s="24">
         <f>DEGREES(ATAN2((SQRT(POWER(K86,2)+POWER(L86,2))),O86))</f>
-        <v>12.506582442617592</v>
+        <v>12.489133495552117</v>
       </c>
       <c r="W86" s="24">
         <f>SQRT(POWER(K86,2)+POWER(L86,2)+POWER(O86,2))</f>
-        <v>6.0587358502648483</v>
+        <v>6.0670659206328352</v>
       </c>
       <c r="X86" s="24">
         <f>DEGREES(ATAN2((SQRT(POWER(K86,2)+POWER(L86,2))),Q86))</f>
-        <v>10.050359677020113</v>
+        <v>10.036177586498006</v>
       </c>
       <c r="Y86" s="25">
         <f>SQRT(POWER(K86,2)+POWER(L86,2)+POWER(Q86,2))</f>
-        <v>6.0071501705288268</v>
+        <v>6.0155516748926976</v>
       </c>
     </row>
     <row r="87" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -7087,7 +7095,8 @@
         <v>1.7529840000000001</v>
       </c>
       <c r="S87" s="23">
-        <v>0</v>
+        <f>DEGREES( ATAN2(L87,K87))</f>
+        <v>-90</v>
       </c>
       <c r="T87" s="24">
         <f>DEGREES(ATAN2((SQRT(POWER(K87,2)+POWER(L87,2))),M87))</f>
@@ -7136,52 +7145,52 @@
         <v>3994.9502779274421</v>
       </c>
       <c r="K88" s="23">
-        <f t="shared" ref="K60:L89" si="20">H88/1000</f>
+        <f t="shared" ref="K60:L89" si="23">H88/1000</f>
         <v>-2.0226463034655597</v>
       </c>
       <c r="L88" s="24">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>3.9949502779274422</v>
       </c>
       <c r="M88" s="25">
-        <f t="shared" ref="M44:M89" si="21">G88/1000</f>
+        <f t="shared" ref="M44:M89" si="24">G88/1000</f>
         <v>0.32300000000000001</v>
       </c>
       <c r="O88" s="31">
-        <f t="shared" ref="O44:O89" si="22">M88-$E$4</f>
+        <f t="shared" ref="O44:O89" si="25">M88-$E$4</f>
         <v>-1.427</v>
       </c>
       <c r="P88" s="10"/>
       <c r="Q88" s="31">
-        <f t="shared" ref="Q44:Q89" si="23">M88-$S$7</f>
+        <f t="shared" ref="Q44:Q89" si="26">M88-$S$7</f>
         <v>-1.6907000000000001</v>
       </c>
       <c r="S88" s="20">
-        <f t="shared" ref="S44:S89" si="24">DEGREES( ATAN2(L88,K88))</f>
+        <f t="shared" ref="S44:S89" si="27">DEGREES( ATAN2(L88,K88))</f>
         <v>-26.853127599364868</v>
       </c>
       <c r="T88" s="21">
-        <f t="shared" ref="T44:T89" si="25">DEGREES(ATAN2((SQRT(POWER(K88,2)+POWER(L88,2))),M88))</f>
+        <f t="shared" ref="T44:T89" si="28">DEGREES(ATAN2((SQRT(POWER(K88,2)+POWER(L88,2))),M88))</f>
         <v>4.1258036033196159</v>
       </c>
       <c r="U88" s="21">
-        <f t="shared" ref="U44:U89" si="26">SQRT(POWER(K88,2)+POWER(L88,2)+POWER(M88,2))</f>
+        <f t="shared" ref="U44:U89" si="29">SQRT(POWER(K88,2)+POWER(L88,2)+POWER(M88,2))</f>
         <v>4.4894381376777472</v>
       </c>
       <c r="V88" s="21">
-        <f t="shared" ref="V44:V89" si="27">DEGREES(ATAN2((SQRT(POWER(K88,2)+POWER(L88,2))),O88))</f>
+        <f t="shared" ref="V44:V89" si="30">DEGREES(ATAN2((SQRT(POWER(K88,2)+POWER(L88,2))),O88))</f>
         <v>-17.676197195270404</v>
       </c>
       <c r="W88" s="21">
-        <f t="shared" ref="W44:W89" si="28">SQRT(POWER(K88,2)+POWER(L88,2)+POWER(O88,2))</f>
+        <f t="shared" ref="W44:W89" si="31">SQRT(POWER(K88,2)+POWER(L88,2)+POWER(O88,2))</f>
         <v>4.6996866695595187</v>
       </c>
       <c r="X88" s="21">
-        <f t="shared" ref="X44:X89" si="29">DEGREES(ATAN2((SQRT(POWER(K88,2)+POWER(L88,2))),Q88))</f>
+        <f t="shared" ref="X44:X89" si="32">DEGREES(ATAN2((SQRT(POWER(K88,2)+POWER(L88,2))),Q88))</f>
         <v>-20.685207470353582</v>
       </c>
       <c r="Y88" s="22">
-        <f t="shared" ref="Y44:Y89" si="30">SQRT(POWER(K88,2)+POWER(L88,2)+POWER(Q88,2))</f>
+        <f t="shared" ref="Y44:Y89" si="33">SQRT(POWER(K88,2)+POWER(L88,2)+POWER(Q88,2))</f>
         <v>4.786354801102342</v>
       </c>
     </row>
@@ -7209,52 +7218,52 @@
         <v>-3994.9502779274421</v>
       </c>
       <c r="K89" s="23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>2.0226463034655597</v>
       </c>
       <c r="L89" s="24">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>-3.9949502779274422</v>
       </c>
       <c r="M89" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0.32300000000000001</v>
       </c>
       <c r="O89" s="32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>-1.427</v>
       </c>
       <c r="P89" s="10"/>
       <c r="Q89" s="32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>-1.6907000000000001</v>
       </c>
       <c r="S89" s="23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>153.14687240063512</v>
       </c>
       <c r="T89" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>4.1258036033196159</v>
       </c>
       <c r="U89" s="24">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>4.4894381376777472</v>
       </c>
       <c r="V89" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>-17.676197195270404</v>
       </c>
       <c r="W89" s="24">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>4.6996866695595187</v>
       </c>
       <c r="X89" s="24">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>-20.685207470353582</v>
       </c>
       <c r="Y89" s="25">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>4.786354801102342</v>
       </c>
     </row>
@@ -19778,7 +19787,7 @@
   <dimension ref="A1:AB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q48" sqref="Q48"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19907,12 +19916,15 @@
       </c>
       <c r="Y2" s="10"/>
       <c r="Z2" s="20">
+        <f>Hufo_SpeakerPositions!S43</f>
         <v>-69.366904439320834</v>
       </c>
       <c r="AA2" s="21">
+        <f>Hufo_SpeakerPositions!X43</f>
         <v>-9.1551706518664009</v>
       </c>
       <c r="AB2" s="22">
+        <f>Hufo_SpeakerPositions!Y43</f>
         <v>6.3729982396428717</v>
       </c>
     </row>
@@ -19995,12 +20007,15 @@
       </c>
       <c r="Y3" s="10"/>
       <c r="Z3" s="20">
+        <f>Hufo_SpeakerPositions!S61</f>
         <v>-69.366904439320834</v>
       </c>
       <c r="AA3" s="21">
+        <f>Hufo_SpeakerPositions!X61</f>
         <v>-2.9387880520458696</v>
       </c>
       <c r="AB3" s="22">
+        <f>Hufo_SpeakerPositions!Y61</f>
         <v>6.3000983772073864</v>
       </c>
     </row>
@@ -20083,12 +20098,15 @@
       </c>
       <c r="Y4" s="10"/>
       <c r="Z4" s="20">
+        <f>Hufo_SpeakerPositions!S79</f>
         <v>-63.423065276213393</v>
       </c>
       <c r="AA4" s="21">
+        <f>Hufo_SpeakerPositions!X79</f>
         <v>10.056999542825952</v>
       </c>
       <c r="AB4" s="22">
+        <f>Hufo_SpeakerPositions!Y79</f>
         <v>6.0032248848066923</v>
       </c>
     </row>
@@ -20171,26 +20189,29 @@
       </c>
       <c r="Y5" s="10"/>
       <c r="Z5" s="20">
+        <f>Hufo_SpeakerPositions!S44</f>
         <v>-55.140915780735916</v>
       </c>
       <c r="AA5" s="21">
+        <f>Hufo_SpeakerPositions!X44</f>
         <v>-10.537158792071354</v>
       </c>
       <c r="AB5" s="22">
+        <f>Hufo_SpeakerPositions!Y44</f>
         <v>5.5448264902700624</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>21</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>20</v>
       </c>
       <c r="F6" s="20">
@@ -20259,12 +20280,15 @@
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="20">
+        <f>Hufo_SpeakerPositions!S62</f>
         <v>-55.140915780735916</v>
       </c>
       <c r="AA6" s="21">
+        <f>Hufo_SpeakerPositions!X62</f>
         <v>-3.3909072024217428</v>
       </c>
       <c r="AB6" s="22">
+        <f>Hufo_SpeakerPositions!Y62</f>
         <v>5.4608821455146437</v>
       </c>
     </row>
@@ -20347,12 +20371,15 @@
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="20">
+        <f>Hufo_SpeakerPositions!S45</f>
         <v>-37.896354740302939</v>
       </c>
       <c r="AA7" s="21">
+        <f>Hufo_SpeakerPositions!X45</f>
         <v>-12.02242380905775</v>
       </c>
       <c r="AB7" s="22">
+        <f>Hufo_SpeakerPositions!Y45</f>
         <v>4.8681076062638029</v>
       </c>
     </row>
@@ -20435,12 +20462,15 @@
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="20">
+        <f>Hufo_SpeakerPositions!S63</f>
         <v>-37.896354740302939</v>
       </c>
       <c r="AA8" s="21">
+        <f>Hufo_SpeakerPositions!X63</f>
         <v>-3.8808947854382496</v>
       </c>
       <c r="AB8" s="22">
+        <f>Hufo_SpeakerPositions!Y63</f>
         <v>4.7722745799213495</v>
       </c>
     </row>
@@ -20523,12 +20553,15 @@
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="20">
+        <f>Hufo_SpeakerPositions!S80</f>
         <v>-25.233336704771727</v>
       </c>
       <c r="AA9" s="21">
+        <f>Hufo_SpeakerPositions!X80</f>
         <v>13.26649045905646</v>
       </c>
       <c r="AB9" s="22">
+        <f>Hufo_SpeakerPositions!Y80</f>
         <v>4.5682742185114842</v>
       </c>
     </row>
@@ -20611,12 +20644,15 @@
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="23">
+        <f>Hufo_SpeakerPositions!S46</f>
         <v>-17.359758769074336</v>
       </c>
       <c r="AA10" s="24">
+        <f>Hufo_SpeakerPositions!X46</f>
         <v>-13.211249325077995</v>
       </c>
       <c r="AB10" s="25">
+        <f>Hufo_SpeakerPositions!Y46</f>
         <v>4.4368209299170784</v>
       </c>
     </row>
@@ -20699,12 +20735,15 @@
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="20">
+        <f>Hufo_SpeakerPositions!S64</f>
         <v>-17.359758769074336</v>
       </c>
       <c r="AA11" s="21">
+        <f>Hufo_SpeakerPositions!X64</f>
         <v>-4.2765598380915124</v>
       </c>
       <c r="AB11" s="22">
+        <f>Hufo_SpeakerPositions!Y64</f>
         <v>4.3314562175035602</v>
       </c>
     </row>
@@ -20787,12 +20826,15 @@
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="20">
+        <f>Hufo_SpeakerPositions!S47</f>
         <v>5.2422918181164526</v>
       </c>
       <c r="AA12" s="21">
+        <f>Hufo_SpeakerPositions!X47</f>
         <v>-13.516063363591293</v>
       </c>
       <c r="AB12" s="22">
+        <f>Hufo_SpeakerPositions!Y47</f>
         <v>4.3385624704556669</v>
       </c>
     </row>
@@ -20875,12 +20917,15 @@
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="20">
+        <f>Hufo_SpeakerPositions!S65</f>
         <v>5.2422918181164526</v>
       </c>
       <c r="AA13" s="21">
+        <f>Hufo_SpeakerPositions!X65</f>
         <v>-4.3785513511579257</v>
       </c>
       <c r="AB13" s="22">
+        <f>Hufo_SpeakerPositions!Y65</f>
         <v>4.2307513883524734</v>
       </c>
     </row>
@@ -20963,26 +21008,29 @@
       </c>
       <c r="Y14" s="10"/>
       <c r="Z14" s="20">
+        <f>Hufo_SpeakerPositions!S81</f>
         <v>24.765206978763871</v>
       </c>
       <c r="AA14" s="21">
+        <f>Hufo_SpeakerPositions!X81</f>
         <v>13.275456050147248</v>
       </c>
       <c r="AB14" s="22">
+        <f>Hufo_SpeakerPositions!Y81</f>
         <v>4.5652443826622653</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <v>30</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>14</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>6</v>
       </c>
       <c r="F15" s="20">
@@ -21051,12 +21099,15 @@
       </c>
       <c r="Y15" s="10"/>
       <c r="Z15" s="20">
+        <f>Hufo_SpeakerPositions!S48</f>
         <v>27.174282601222639</v>
       </c>
       <c r="AA15" s="21">
+        <f>Hufo_SpeakerPositions!X48</f>
         <v>-12.740971812728684</v>
       </c>
       <c r="AB15" s="22">
+        <f>Hufo_SpeakerPositions!Y48</f>
         <v>4.5977272909007176</v>
       </c>
     </row>
@@ -21139,12 +21190,15 @@
       </c>
       <c r="Y16" s="10"/>
       <c r="Z16" s="20">
+        <f>Hufo_SpeakerPositions!S66</f>
         <v>27.174282601222639</v>
       </c>
       <c r="AA16" s="21">
+        <f>Hufo_SpeakerPositions!X66</f>
         <v>-4.1196477900941169</v>
       </c>
       <c r="AB16" s="22">
+        <f>Hufo_SpeakerPositions!Y66</f>
         <v>4.496134922518813</v>
       </c>
     </row>
@@ -21227,12 +21281,15 @@
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="20">
+        <f>Hufo_SpeakerPositions!S49</f>
         <v>46.237789767953686</v>
       </c>
       <c r="AA17" s="21">
+        <f>Hufo_SpeakerPositions!X49</f>
         <v>-11.346448197505596</v>
       </c>
       <c r="AB17" s="22">
+        <f>Hufo_SpeakerPositions!Y49</f>
         <v>5.1539831620794558</v>
       </c>
     </row>
@@ -21315,12 +21372,15 @@
       </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="20">
+        <f>Hufo_SpeakerPositions!S67</f>
         <v>46.237789767953686</v>
       </c>
       <c r="AA18" s="21">
+        <f>Hufo_SpeakerPositions!X67</f>
         <v>-3.6573275784143031</v>
       </c>
       <c r="AB18" s="22">
+        <f>Hufo_SpeakerPositions!Y67</f>
         <v>5.063563511500428</v>
       </c>
     </row>
@@ -21403,12 +21463,15 @@
       </c>
       <c r="Y19" s="10"/>
       <c r="Z19" s="23">
+        <f>Hufo_SpeakerPositions!S50</f>
         <v>62.014206415626006</v>
       </c>
       <c r="AA19" s="24">
+        <f>Hufo_SpeakerPositions!X50</f>
         <v>-9.8783589719401519</v>
       </c>
       <c r="AB19" s="25">
+        <f>Hufo_SpeakerPositions!Y50</f>
         <v>5.9105718191941428</v>
       </c>
     </row>
@@ -21491,12 +21554,15 @@
       </c>
       <c r="Y20" s="10"/>
       <c r="Z20" s="20">
+        <f>Hufo_SpeakerPositions!S68</f>
         <v>62.014206415626006</v>
       </c>
       <c r="AA20" s="21">
+        <f>Hufo_SpeakerPositions!X68</f>
         <v>-3.1749565589924145</v>
       </c>
       <c r="AB20" s="22">
+        <f>Hufo_SpeakerPositions!Y68</f>
         <v>5.8318943946072928</v>
       </c>
     </row>
@@ -21579,12 +21645,15 @@
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="20">
+        <f>Hufo_SpeakerPositions!S82</f>
         <v>63.615252451855795</v>
       </c>
       <c r="AA21" s="21">
+        <f>Hufo_SpeakerPositions!X82</f>
         <v>10.036177586498006</v>
       </c>
       <c r="AB21" s="22">
+        <f>Hufo_SpeakerPositions!Y82</f>
         <v>6.0155516748926976</v>
       </c>
     </row>
@@ -21667,12 +21736,15 @@
       </c>
       <c r="Y22" s="10"/>
       <c r="Z22" s="20">
+        <f>Hufo_SpeakerPositions!S51</f>
         <v>75.44454726885877</v>
       </c>
       <c r="AA22" s="21">
+        <f>Hufo_SpeakerPositions!X51</f>
         <v>-8.5635721303178229</v>
       </c>
       <c r="AB22" s="22">
+        <f>Hufo_SpeakerPositions!Y51</f>
         <v>6.809634264874334</v>
       </c>
     </row>
@@ -21755,12 +21827,15 @@
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="20">
+        <f>Hufo_SpeakerPositions!S69</f>
         <v>75.44454726885877</v>
       </c>
       <c r="AA23" s="21">
+        <f>Hufo_SpeakerPositions!X69</f>
         <v>-2.7462346530811899</v>
       </c>
       <c r="AB23" s="22">
+        <f>Hufo_SpeakerPositions!Y69</f>
         <v>6.7414576926174208</v>
       </c>
     </row>
@@ -21843,12 +21918,15 @@
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="20">
+        <f>Hufo_SpeakerPositions!S52</f>
         <v>110.63309556067915</v>
       </c>
       <c r="AA24" s="21">
+        <f>Hufo_SpeakerPositions!X52</f>
         <v>-9.1551706518664009</v>
       </c>
       <c r="AB24" s="22">
+        <f>Hufo_SpeakerPositions!Y52</f>
         <v>6.3729982396428717</v>
       </c>
     </row>
@@ -21931,12 +22009,15 @@
       </c>
       <c r="Y25" s="10"/>
       <c r="Z25" s="20">
+        <f>Hufo_SpeakerPositions!S70</f>
         <v>110.63309556067915</v>
       </c>
       <c r="AA25" s="21">
+        <f>Hufo_SpeakerPositions!X70</f>
         <v>-2.9387880520458696</v>
       </c>
       <c r="AB25" s="22">
+        <f>Hufo_SpeakerPositions!Y70</f>
         <v>6.3000983772073864</v>
       </c>
     </row>
@@ -21955,11 +22036,11 @@
       </c>
       <c r="F26" s="20">
         <f>Hufo_SpeakerPositions!K83</f>
-        <v>-5.2838320181506457</v>
+        <v>5.2863950181506461</v>
       </c>
       <c r="G26" s="21">
         <f>Hufo_SpeakerPositions!L83</f>
-        <v>2.6461271955159247</v>
+        <v>-2.6445681955159244</v>
       </c>
       <c r="H26" s="22">
         <f>Hufo_SpeakerPositions!M83</f>
@@ -21968,11 +22049,11 @@
       <c r="I26" s="10"/>
       <c r="J26" s="20">
         <f>Hufo_SpeakerPositions!K83</f>
-        <v>-5.2838320181506457</v>
+        <v>5.2863950181506461</v>
       </c>
       <c r="K26" s="21">
         <f>Hufo_SpeakerPositions!L83</f>
-        <v>2.6461271955159247</v>
+        <v>-2.6445681955159244</v>
       </c>
       <c r="L26" s="31">
         <f>Hufo_SpeakerPositions!O83</f>
@@ -21981,11 +22062,11 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10">
         <f>Hufo_SpeakerPositions!K83</f>
-        <v>-5.2838320181506457</v>
+        <v>5.2863950181506461</v>
       </c>
       <c r="O26" s="10">
         <f>Hufo_SpeakerPositions!L83</f>
-        <v>2.6461271955159247</v>
+        <v>-2.6445681955159244</v>
       </c>
       <c r="P26" s="10">
         <f>Hufo_SpeakerPositions!Q83</f>
@@ -21994,38 +22075,41 @@
       <c r="Q26" s="10"/>
       <c r="R26" s="20">
         <f>Hufo_SpeakerPositions!S83</f>
-        <v>-63.398428921421988</v>
+        <v>116.57693472378661</v>
       </c>
       <c r="S26" s="21">
         <f>Hufo_SpeakerPositions!T83</f>
-        <v>27.391547369746746</v>
+        <v>27.385235002966883</v>
       </c>
       <c r="T26" s="21">
         <f>Hufo_SpeakerPositions!U83</f>
-        <v>6.6555914576980237</v>
+        <v>6.6570069062276271</v>
       </c>
       <c r="U26" s="10"/>
       <c r="V26" s="10">
         <f>Hufo_SpeakerPositions!S83</f>
-        <v>-63.398428921421988</v>
+        <v>116.57693472378661</v>
       </c>
       <c r="W26" s="10">
         <f>Hufo_SpeakerPositions!V83</f>
-        <v>12.518021148079114</v>
+        <v>12.514751523165046</v>
       </c>
       <c r="X26" s="10">
         <f>Hufo_SpeakerPositions!W83</f>
-        <v>6.0532877555740647</v>
+        <v>6.0548440070378629</v>
       </c>
       <c r="Y26" s="10"/>
       <c r="Z26" s="20">
-        <v>-63.398428921421988</v>
+        <f>Hufo_SpeakerPositions!S83</f>
+        <v>116.57693472378661</v>
       </c>
       <c r="AA26" s="21">
-        <v>10.059657150098166</v>
+        <f>Hufo_SpeakerPositions!X83</f>
+        <v>10.056999542825952</v>
       </c>
       <c r="AB26" s="22">
-        <v>6.0016552483279897</v>
+        <f>Hufo_SpeakerPositions!Y83</f>
+        <v>6.0032248848066923</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
@@ -22107,12 +22191,15 @@
       </c>
       <c r="Y27" s="10"/>
       <c r="Z27" s="20">
+        <f>Hufo_SpeakerPositions!S53</f>
         <v>124.85908421926409</v>
       </c>
       <c r="AA27" s="21">
+        <f>Hufo_SpeakerPositions!X53</f>
         <v>-10.537158792071354</v>
       </c>
       <c r="AB27" s="22">
+        <f>Hufo_SpeakerPositions!Y53</f>
         <v>5.5448264902700624</v>
       </c>
     </row>
@@ -22195,12 +22282,15 @@
       </c>
       <c r="Y28" s="10"/>
       <c r="Z28" s="23">
+        <f>Hufo_SpeakerPositions!S71</f>
         <v>124.85908421926409</v>
       </c>
       <c r="AA28" s="24">
+        <f>Hufo_SpeakerPositions!X71</f>
         <v>-3.3909072024217428</v>
       </c>
       <c r="AB28" s="25">
+        <f>Hufo_SpeakerPositions!Y71</f>
         <v>5.4608821455146437</v>
       </c>
     </row>
@@ -22283,12 +22373,15 @@
       </c>
       <c r="Y29" s="10"/>
       <c r="Z29" s="20">
+        <f>Hufo_SpeakerPositions!S54</f>
         <v>142.10364525969706</v>
       </c>
       <c r="AA29" s="21">
+        <f>Hufo_SpeakerPositions!X54</f>
         <v>-12.02242380905775</v>
       </c>
       <c r="AB29" s="22">
+        <f>Hufo_SpeakerPositions!Y54</f>
         <v>4.8681076062638029</v>
       </c>
     </row>
@@ -22371,12 +22464,15 @@
       </c>
       <c r="Y30" s="10"/>
       <c r="Z30" s="20">
+        <f>Hufo_SpeakerPositions!S72</f>
         <v>142.10364525969706</v>
       </c>
       <c r="AA30" s="21">
+        <f>Hufo_SpeakerPositions!X72</f>
         <v>-3.8808947854382496</v>
       </c>
       <c r="AB30" s="22">
+        <f>Hufo_SpeakerPositions!Y72</f>
         <v>4.7722745799213495</v>
       </c>
     </row>
@@ -22395,11 +22491,11 @@
       </c>
       <c r="F31" s="20">
         <f>Hufo_SpeakerPositions!K84</f>
-        <v>-1.8387873034655597</v>
+        <v>1.8955093034655597</v>
       </c>
       <c r="G31" s="21">
         <f>Hufo_SpeakerPositions!L84</f>
-        <v>4.0341932779274421</v>
+        <v>-4.0220862779274418</v>
       </c>
       <c r="H31" s="22">
         <f>Hufo_SpeakerPositions!M84</f>
@@ -22408,11 +22504,11 @@
       <c r="I31" s="10"/>
       <c r="J31" s="20">
         <f>Hufo_SpeakerPositions!K84</f>
-        <v>-1.8387873034655597</v>
+        <v>1.8955093034655597</v>
       </c>
       <c r="K31" s="21">
         <f>Hufo_SpeakerPositions!L84</f>
-        <v>4.0341932779274421</v>
+        <v>-4.0220862779274418</v>
       </c>
       <c r="L31" s="31">
         <f>Hufo_SpeakerPositions!O84</f>
@@ -22421,11 +22517,11 @@
       <c r="M31" s="10"/>
       <c r="N31" s="10">
         <f>Hufo_SpeakerPositions!K84</f>
-        <v>-1.8387873034655597</v>
+        <v>1.8955093034655597</v>
       </c>
       <c r="O31" s="10">
         <f>Hufo_SpeakerPositions!L84</f>
-        <v>4.0341932779274421</v>
+        <v>-4.0220862779274418</v>
       </c>
       <c r="P31" s="10">
         <f>Hufo_SpeakerPositions!Q84</f>
@@ -22434,38 +22530,41 @@
       <c r="Q31" s="10"/>
       <c r="R31" s="20">
         <f>Hufo_SpeakerPositions!S84</f>
-        <v>-24.503522137434636</v>
+        <v>154.76666329522828</v>
       </c>
       <c r="S31" s="21">
         <f>Hufo_SpeakerPositions!T84</f>
-        <v>34.631235178960253</v>
+        <v>34.553616538294953</v>
       </c>
       <c r="T31" s="21">
         <f>Hufo_SpeakerPositions!U84</f>
-        <v>5.3881241514984701</v>
+        <v>5.398718483817869</v>
       </c>
       <c r="U31" s="10"/>
       <c r="V31" s="10">
         <f>Hufo_SpeakerPositions!S84</f>
-        <v>-24.503522137434636</v>
+        <v>154.76666329522828</v>
       </c>
       <c r="W31" s="10">
         <f>Hufo_SpeakerPositions!V84</f>
-        <v>16.485382316912638</v>
+        <v>16.440246799953421</v>
       </c>
       <c r="X31" s="10">
         <f>Hufo_SpeakerPositions!W84</f>
-        <v>4.6235567339399122</v>
+        <v>4.6358986472437804</v>
       </c>
       <c r="Y31" s="10"/>
       <c r="Z31" s="20">
-        <v>-24.503522137434636</v>
+        <f>Hufo_SpeakerPositions!S84</f>
+        <v>154.76666329522828</v>
       </c>
       <c r="AA31" s="21">
-        <v>13.303632931919649</v>
+        <f>Hufo_SpeakerPositions!X84</f>
+        <v>13.26649045905646</v>
       </c>
       <c r="AB31" s="22">
-        <v>4.5557491085397919</v>
+        <f>Hufo_SpeakerPositions!Y84</f>
+        <v>4.5682742185114842</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
@@ -22475,10 +22574,10 @@
       <c r="B32" s="19">
         <v>25</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>9</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>13</v>
       </c>
       <c r="F32" s="20">
@@ -22547,12 +22646,15 @@
       </c>
       <c r="Y32" s="10"/>
       <c r="Z32" s="20">
+        <f>Hufo_SpeakerPositions!S55</f>
         <v>162.64024123092568</v>
       </c>
       <c r="AA32" s="21">
+        <f>Hufo_SpeakerPositions!X55</f>
         <v>-13.211249325077995</v>
       </c>
       <c r="AB32" s="22">
+        <f>Hufo_SpeakerPositions!Y55</f>
         <v>4.4368209299170784</v>
       </c>
     </row>
@@ -22635,12 +22737,15 @@
       </c>
       <c r="Y33" s="10"/>
       <c r="Z33" s="20">
+        <f>Hufo_SpeakerPositions!S73</f>
         <v>162.64024123092568</v>
       </c>
       <c r="AA33" s="21">
+        <f>Hufo_SpeakerPositions!X73</f>
         <v>-4.2765598380915124</v>
       </c>
       <c r="AB33" s="22">
+        <f>Hufo_SpeakerPositions!Y73</f>
         <v>4.3314562175035602</v>
       </c>
     </row>
@@ -22723,12 +22828,15 @@
       </c>
       <c r="Y34" s="10"/>
       <c r="Z34" s="20">
+        <f>Hufo_SpeakerPositions!S56</f>
         <v>-174.75770818188354</v>
       </c>
       <c r="AA34" s="21">
+        <f>Hufo_SpeakerPositions!X56</f>
         <v>-13.516063363591293</v>
       </c>
       <c r="AB34" s="22">
+        <f>Hufo_SpeakerPositions!Y56</f>
         <v>4.3385624704556669</v>
       </c>
     </row>
@@ -22811,12 +22919,15 @@
       </c>
       <c r="Y35" s="10"/>
       <c r="Z35" s="20">
+        <f>Hufo_SpeakerPositions!S74</f>
         <v>-174.75770818188354</v>
       </c>
       <c r="AA35" s="21">
+        <f>Hufo_SpeakerPositions!X74</f>
         <v>-4.3785513511579257</v>
       </c>
       <c r="AB35" s="22">
+        <f>Hufo_SpeakerPositions!Y74</f>
         <v>4.2307513883524734</v>
       </c>
     </row>
@@ -22835,11 +22946,11 @@
       </c>
       <c r="F36" s="20">
         <f>Hufo_SpeakerPositions!K85</f>
-        <v>1.8387873034655597</v>
+        <v>-1.8612803034655598</v>
       </c>
       <c r="G36" s="21">
         <f>Hufo_SpeakerPositions!L85</f>
-        <v>4.0396219999999996</v>
+        <v>-4.034612263459838</v>
       </c>
       <c r="H36" s="22">
         <f>Hufo_SpeakerPositions!M85</f>
@@ -22848,11 +22959,11 @@
       <c r="I36" s="10"/>
       <c r="J36" s="20">
         <f>Hufo_SpeakerPositions!K85</f>
-        <v>1.8387873034655597</v>
+        <v>-1.8612803034655598</v>
       </c>
       <c r="K36" s="21">
         <f>Hufo_SpeakerPositions!L85</f>
-        <v>4.0396219999999996</v>
+        <v>-4.034612263459838</v>
       </c>
       <c r="L36" s="31">
         <f>Hufo_SpeakerPositions!O85</f>
@@ -22861,11 +22972,11 @@
       <c r="M36" s="10"/>
       <c r="N36" s="10">
         <f>Hufo_SpeakerPositions!K85</f>
-        <v>1.8387873034655597</v>
+        <v>-1.8612803034655598</v>
       </c>
       <c r="O36" s="10">
         <f>Hufo_SpeakerPositions!L85</f>
-        <v>4.0396219999999996</v>
+        <v>-4.034612263459838</v>
       </c>
       <c r="P36" s="10">
         <f>Hufo_SpeakerPositions!Q85</f>
@@ -22874,38 +22985,41 @@
       <c r="Q36" s="10"/>
       <c r="R36" s="20">
         <f>Hufo_SpeakerPositions!S85</f>
-        <v>24.47445674721007</v>
+        <v>-155.23479302123613</v>
       </c>
       <c r="S36" s="21">
         <f>Hufo_SpeakerPositions!T85</f>
-        <v>34.601402800999509</v>
+        <v>34.572363524646619</v>
       </c>
       <c r="T36" s="21">
         <f>Hufo_SpeakerPositions!U85</f>
-        <v>5.3921899420523145</v>
+        <v>5.3961549463881564</v>
       </c>
       <c r="U36" s="10"/>
       <c r="V36" s="10">
         <f>Hufo_SpeakerPositions!S85</f>
-        <v>24.47445674721007</v>
+        <v>-155.23479302123613</v>
       </c>
       <c r="W36" s="10">
         <f>Hufo_SpeakerPositions!V85</f>
-        <v>16.468027189366833</v>
+        <v>16.451142441190825</v>
       </c>
       <c r="X36" s="10">
         <f>Hufo_SpeakerPositions!W85</f>
-        <v>4.628294218302262</v>
+        <v>4.6329130366789064</v>
       </c>
       <c r="Y36" s="10"/>
       <c r="Z36" s="20">
-        <v>24.47445674721007</v>
+        <f>Hufo_SpeakerPositions!S85</f>
+        <v>-155.23479302123613</v>
       </c>
       <c r="AA36" s="21">
-        <v>13.289350521250501</v>
+        <f>Hufo_SpeakerPositions!X85</f>
+        <v>13.275456050147248</v>
       </c>
       <c r="AB36" s="22">
-        <v>4.5605570316760806</v>
+        <f>Hufo_SpeakerPositions!Y85</f>
+        <v>4.5652443826622653</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.2">
@@ -22987,12 +23101,15 @@
       </c>
       <c r="Y37" s="10"/>
       <c r="Z37" s="23">
+        <f>Hufo_SpeakerPositions!S57</f>
         <v>-152.82571739877736</v>
       </c>
       <c r="AA37" s="24">
+        <f>Hufo_SpeakerPositions!X57</f>
         <v>-12.740971812728684</v>
       </c>
       <c r="AB37" s="25">
+        <f>Hufo_SpeakerPositions!Y57</f>
         <v>4.5977272909007176</v>
       </c>
     </row>
@@ -23075,12 +23192,15 @@
       </c>
       <c r="Y38" s="10"/>
       <c r="Z38" s="20">
+        <f>Hufo_SpeakerPositions!S75</f>
         <v>-152.82571739877736</v>
       </c>
       <c r="AA38" s="21">
+        <f>Hufo_SpeakerPositions!X75</f>
         <v>-4.1196477900941169</v>
       </c>
       <c r="AB38" s="22">
+        <f>Hufo_SpeakerPositions!Y75</f>
         <v>4.496134922518813</v>
       </c>
     </row>
@@ -23163,12 +23283,15 @@
       </c>
       <c r="Y39" s="10"/>
       <c r="Z39" s="20">
+        <f>Hufo_SpeakerPositions!S58</f>
         <v>-133.7622102320463</v>
       </c>
       <c r="AA39" s="21">
+        <f>Hufo_SpeakerPositions!X58</f>
         <v>-11.346448197505596</v>
       </c>
       <c r="AB39" s="22">
+        <f>Hufo_SpeakerPositions!Y58</f>
         <v>5.1539831620794558</v>
       </c>
     </row>
@@ -23251,12 +23374,15 @@
       </c>
       <c r="Y40" s="10"/>
       <c r="Z40" s="20">
+        <f>Hufo_SpeakerPositions!S76</f>
         <v>-133.7622102320463</v>
       </c>
       <c r="AA40" s="21">
+        <f>Hufo_SpeakerPositions!X76</f>
         <v>-3.6573275784143031</v>
       </c>
       <c r="AB40" s="22">
+        <f>Hufo_SpeakerPositions!Y76</f>
         <v>5.063563511500428</v>
       </c>
     </row>
@@ -23339,12 +23465,15 @@
       </c>
       <c r="Y41" s="10"/>
       <c r="Z41" s="23">
+        <f>Hufo_SpeakerPositions!S59</f>
         <v>-117.98579358437399</v>
       </c>
       <c r="AA41" s="24">
+        <f>Hufo_SpeakerPositions!X59</f>
         <v>-9.8783589719401519</v>
       </c>
       <c r="AB41" s="25">
+        <f>Hufo_SpeakerPositions!Y59</f>
         <v>5.9105718191941428</v>
       </c>
     </row>
@@ -23427,12 +23556,15 @@
       </c>
       <c r="Y42" s="10"/>
       <c r="Z42" s="20">
+        <f>Hufo_SpeakerPositions!S77</f>
         <v>-117.98579358437399</v>
       </c>
       <c r="AA42" s="21">
+        <f>Hufo_SpeakerPositions!X77</f>
         <v>-3.1749565589924145</v>
       </c>
       <c r="AB42" s="22">
+        <f>Hufo_SpeakerPositions!Y77</f>
         <v>5.8318943946072928</v>
       </c>
     </row>
@@ -23451,11 +23583,11 @@
       </c>
       <c r="F43" s="20">
         <f>Hufo_SpeakerPositions!K86</f>
-        <v>5.2927826070532085</v>
+        <v>-5.3064506070532076</v>
       </c>
       <c r="G43" s="21">
         <f>Hufo_SpeakerPositions!L86</f>
-        <v>2.6407024930611844</v>
+        <v>-2.6323844930611839</v>
       </c>
       <c r="H43" s="22">
         <f>Hufo_SpeakerPositions!M86</f>
@@ -23464,11 +23596,11 @@
       <c r="I43" s="10"/>
       <c r="J43" s="20">
         <f>Hufo_SpeakerPositions!K86</f>
-        <v>5.2927826070532085</v>
+        <v>-5.3064506070532076</v>
       </c>
       <c r="K43" s="21">
         <f>Hufo_SpeakerPositions!L86</f>
-        <v>2.6407024930611844</v>
+        <v>-2.6323844930611839</v>
       </c>
       <c r="L43" s="31">
         <f>Hufo_SpeakerPositions!O86</f>
@@ -23477,11 +23609,11 @@
       <c r="M43" s="10"/>
       <c r="N43" s="10">
         <f>Hufo_SpeakerPositions!K86</f>
-        <v>5.2927826070532085</v>
+        <v>-5.3064506070532076</v>
       </c>
       <c r="O43" s="10">
         <f>Hufo_SpeakerPositions!L86</f>
-        <v>2.6407024930611844</v>
+        <v>-2.6323844930611839</v>
       </c>
       <c r="P43" s="10">
         <f>Hufo_SpeakerPositions!Q86</f>
@@ -23490,38 +23622,41 @@
       <c r="Q43" s="10"/>
       <c r="R43" s="20">
         <f>Hufo_SpeakerPositions!S86</f>
-        <v>63.484236310055316</v>
+        <v>-116.3847475481442</v>
       </c>
       <c r="S43" s="21">
         <f>Hufo_SpeakerPositions!T86</f>
-        <v>27.369461253572339</v>
+        <v>27.335757209509374</v>
       </c>
       <c r="T43" s="21">
         <f>Hufo_SpeakerPositions!U86</f>
-        <v>6.6605469072204961</v>
+        <v>6.6681252151788772</v>
       </c>
       <c r="U43" s="10"/>
       <c r="V43" s="10">
         <f>Hufo_SpeakerPositions!S86</f>
-        <v>63.484236310055316</v>
+        <v>-116.3847475481442</v>
       </c>
       <c r="W43" s="10">
         <f>Hufo_SpeakerPositions!V86</f>
-        <v>12.506582442617592</v>
+        <v>12.489133495552117</v>
       </c>
       <c r="X43" s="10">
         <f>Hufo_SpeakerPositions!W86</f>
-        <v>6.0587358502648483</v>
+        <v>6.0670659206328352</v>
       </c>
       <c r="Y43" s="10"/>
       <c r="Z43" s="20">
-        <v>63.484236310055316</v>
+        <f>Hufo_SpeakerPositions!S86</f>
+        <v>-116.3847475481442</v>
       </c>
       <c r="AA43" s="21">
-        <v>10.050359677020113</v>
+        <f>Hufo_SpeakerPositions!X86</f>
+        <v>10.036177586498006</v>
       </c>
       <c r="AB43" s="22">
-        <v>6.0071501705288268</v>
+        <f>Hufo_SpeakerPositions!Y86</f>
+        <v>6.0155516748926976</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.2">
@@ -23603,12 +23738,15 @@
       </c>
       <c r="Y44" s="10"/>
       <c r="Z44" s="20">
+        <f>Hufo_SpeakerPositions!S60</f>
         <v>-104.55545273114123</v>
       </c>
       <c r="AA44" s="21">
+        <f>Hufo_SpeakerPositions!X60</f>
         <v>-8.5635721303178229</v>
       </c>
       <c r="AB44" s="22">
+        <f>Hufo_SpeakerPositions!Y60</f>
         <v>6.809634264874334</v>
       </c>
     </row>
@@ -23691,12 +23829,15 @@
       </c>
       <c r="Y45" s="10"/>
       <c r="Z45" s="23">
+        <f>Hufo_SpeakerPositions!S78</f>
         <v>-104.55545273114123</v>
       </c>
       <c r="AA45" s="24">
+        <f>Hufo_SpeakerPositions!X78</f>
         <v>-2.7462346530811899</v>
       </c>
       <c r="AB45" s="25">
+        <f>Hufo_SpeakerPositions!Y78</f>
         <v>6.7414576926174208</v>
       </c>
     </row>
@@ -23754,7 +23895,7 @@
       <c r="Q46" s="10"/>
       <c r="R46" s="10">
         <f>Hufo_SpeakerPositions!S87</f>
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="S46" s="10">
         <f>Hufo_SpeakerPositions!T87</f>
@@ -23767,7 +23908,7 @@
       <c r="U46" s="10"/>
       <c r="V46" s="23">
         <f>Hufo_SpeakerPositions!$S$87</f>
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="W46" s="24">
         <f>Hufo_SpeakerPositions!$V$87</f>
@@ -23779,15 +23920,15 @@
       </c>
       <c r="Y46" s="10"/>
       <c r="Z46" s="10">
-        <f>Hufo_SpeakerPositions!$S$87</f>
-        <v>0</v>
+        <f>Hufo_SpeakerPositions!S87</f>
+        <v>-90</v>
       </c>
       <c r="AA46" s="10">
-        <f>Hufo_SpeakerPositions!$X$87</f>
+        <f>Hufo_SpeakerPositions!X87</f>
         <v>80.28866454423698</v>
       </c>
       <c r="AB46" s="10">
-        <f>Hufo_SpeakerPositions!$Y$87</f>
+        <f>Hufo_SpeakerPositions!Y87</f>
         <v>1.7784692587323516</v>
       </c>
     </row>
@@ -23818,6 +23959,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB45">
     <sortCondition ref="A2:A45"/>
     <sortCondition ref="B2:B45"/>
+    <sortCondition ref="D2:D45"/>
   </sortState>
   <mergeCells count="6">
     <mergeCell ref="F1:H1"/>
@@ -23837,630 +23979,631 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C45"/>
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1">
+      <c r="A1" s="3">
         <f>SortedSpeaker!R2</f>
         <v>-69.366904439320834</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
         <f>SortedSpeaker!S2</f>
         <v>9.0282006154422199</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="3">
         <f>SortedSpeaker!T2</f>
         <v>6.3707386269169088</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="3">
         <f>SortedSpeaker!R3</f>
         <v>-69.366904439320834</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <f>SortedSpeaker!S3</f>
         <v>15.040892032043063</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <f>SortedSpeaker!T3</f>
         <v>6.5150116694055997</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="3">
         <f>SortedSpeaker!R4</f>
         <v>-63.423065276213393</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <f>SortedSpeaker!S4</f>
         <v>27.385235002966883</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <f>SortedSpeaker!T4</f>
         <v>6.6570069062276271</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="3">
         <f>SortedSpeaker!R5</f>
         <v>-55.140915780735916</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <f>SortedSpeaker!S5</f>
         <v>10.391817680761241</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <f>SortedSpeaker!T5</f>
         <v>5.5422292353529201</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="3">
         <f>SortedSpeaker!R6</f>
         <v>-55.140915780735916</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <f>SortedSpeaker!S6</f>
         <v>17.231014707876284</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f>SortedSpeaker!T6</f>
         <v>5.7074837973664554</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="3">
         <f>SortedSpeaker!R7</f>
         <v>-37.896354740302939</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <f>SortedSpeaker!S7</f>
         <v>11.857709493933276</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f>SortedSpeaker!T7</f>
         <v>4.8651490990681356</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="3">
         <f>SortedSpeaker!R8</f>
         <v>-37.896354740302939</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <f>SortedSpeaker!S8</f>
         <v>19.549429629941635</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <f>SortedSpeaker!T8</f>
         <v>5.0525975652295418</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="3">
         <f>SortedSpeaker!R9</f>
         <v>-25.233336704771727</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <f>SortedSpeaker!S9</f>
         <v>34.553616538294953</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <f>SortedSpeaker!T9</f>
         <v>5.398718483817869</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
         <f>SortedSpeaker!R10</f>
         <v>-17.359758769074336</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <f>SortedSpeaker!S10</f>
         <v>13.031338827122806</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <f>SortedSpeaker!T10</f>
         <v>4.4335746361316906</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <f>SortedSpeaker!R11</f>
         <v>-17.359758769074336</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <f>SortedSpeaker!S11</f>
         <v>21.376390611636417</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <f>SortedSpeaker!T11</f>
         <v>4.6384965726138301</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="3">
         <f>SortedSpeaker!R12</f>
         <v>5.2422918181164526</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <f>SortedSpeaker!S12</f>
         <v>13.332304509064471</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <f>SortedSpeaker!T12</f>
         <v>4.335242599906767</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="3">
         <f>SortedSpeaker!R13</f>
         <v>5.2422918181164526</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <f>SortedSpeaker!S13</f>
         <v>21.840490063843184</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <f>SortedSpeaker!T13</f>
         <v>4.5446006205217175</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="3">
         <f>SortedSpeaker!R14</f>
         <v>24.765206978763871</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <f>SortedSpeaker!S14</f>
         <v>34.572363524646619</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <f>SortedSpeaker!T14</f>
         <v>5.3961549463881564</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="3">
         <f>SortedSpeaker!R15</f>
         <v>27.174282601222639</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <f>SortedSpeaker!S15</f>
         <v>12.56703773496713</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <f>SortedSpeaker!T15</f>
         <v>4.5945946863127389</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="3">
         <f>SortedSpeaker!R16</f>
         <v>27.174282601222639</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <f>SortedSpeaker!S16</f>
         <v>20.656854314257824</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <f>SortedSpeaker!T16</f>
         <v>4.7926367201670166</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="3">
         <f>SortedSpeaker!R17</f>
         <v>46.237789767953686</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <f>SortedSpeaker!S17</f>
         <v>11.19050026689353</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <f>SortedSpeaker!T17</f>
         <v>5.1511888457907027</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="3">
         <f>SortedSpeaker!R18</f>
         <v>46.237789767953686</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <f>SortedSpeaker!S18</f>
         <v>18.499039879728343</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <f>SortedSpeaker!T18</f>
         <v>5.3285845142024861</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="3">
         <f>SortedSpeaker!R19</f>
         <v>62.014206415626006</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <f>SortedSpeaker!S19</f>
         <v>9.7417366465724218</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <f>SortedSpeaker!T19</f>
         <v>5.9081353505020484</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="3">
         <f>SortedSpeaker!R20</f>
         <v>62.014206415626006</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <f>SortedSpeaker!S20</f>
         <v>16.19073271223106</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <f>SortedSpeaker!T20</f>
         <v>6.0634255763431248</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="3">
         <f>SortedSpeaker!R21</f>
         <v>63.615252451855795</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <f>SortedSpeaker!S21</f>
         <v>27.335757209509374</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <f>SortedSpeaker!T21</f>
         <v>6.6681252151788772</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="3">
         <f>SortedSpeaker!R22</f>
         <v>75.44454726885877</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <f>SortedSpeaker!S22</f>
         <v>8.4445573083844039</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <f>SortedSpeaker!T22</f>
         <v>6.8075195858220345</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="3">
         <f>SortedSpeaker!R23</f>
         <v>75.44454726885877</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <f>SortedSpeaker!S23</f>
         <v>14.094458060134764</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <f>SortedSpeaker!T23</f>
         <v>6.9427220390384781</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="3">
         <f>SortedSpeaker!R24</f>
         <v>110.63309556067915</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <f>SortedSpeaker!S24</f>
         <v>9.0282006154422199</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <f>SortedSpeaker!T24</f>
         <v>6.3707386269169088</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="3">
         <f>SortedSpeaker!R25</f>
         <v>110.63309556067915</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <f>SortedSpeaker!S25</f>
         <v>15.040892032043063</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <f>SortedSpeaker!T25</f>
         <v>6.5150116694055997</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="3">
         <f>SortedSpeaker!R26</f>
-        <v>-63.398428921421988</v>
-      </c>
-      <c r="B25">
+        <v>116.57693472378661</v>
+      </c>
+      <c r="B25" s="3">
         <f>SortedSpeaker!S26</f>
-        <v>27.391547369746746</v>
-      </c>
-      <c r="C25">
+        <v>27.385235002966883</v>
+      </c>
+      <c r="C25" s="3">
         <f>SortedSpeaker!T26</f>
-        <v>6.6555914576980237</v>
+        <v>6.6570069062276271</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="3">
         <f>SortedSpeaker!R27</f>
         <v>124.85908421926409</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <f>SortedSpeaker!S27</f>
         <v>10.391817680761241</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <f>SortedSpeaker!T27</f>
         <v>5.5422292353529201</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="3">
         <f>SortedSpeaker!R28</f>
         <v>124.85908421926409</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <f>SortedSpeaker!S28</f>
         <v>17.231014707876284</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <f>SortedSpeaker!T28</f>
         <v>5.7074837973664554</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="3">
         <f>SortedSpeaker!R29</f>
         <v>142.10364525969706</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <f>SortedSpeaker!S29</f>
         <v>11.857709493933276</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <f>SortedSpeaker!T29</f>
         <v>4.8651490990681356</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="3">
         <f>SortedSpeaker!R30</f>
         <v>142.10364525969706</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <f>SortedSpeaker!S30</f>
         <v>19.549429629941635</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <f>SortedSpeaker!T30</f>
         <v>5.0525975652295418</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="3">
         <f>SortedSpeaker!R31</f>
-        <v>-24.503522137434636</v>
-      </c>
-      <c r="B30">
+        <v>154.76666329522828</v>
+      </c>
+      <c r="B30" s="3">
         <f>SortedSpeaker!S31</f>
-        <v>34.631235178960253</v>
-      </c>
-      <c r="C30">
+        <v>34.553616538294953</v>
+      </c>
+      <c r="C30" s="3">
         <f>SortedSpeaker!T31</f>
-        <v>5.3881241514984701</v>
+        <v>5.398718483817869</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="3">
         <f>SortedSpeaker!R32</f>
         <v>162.64024123092568</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <f>SortedSpeaker!S32</f>
         <v>13.031338827122806</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <f>SortedSpeaker!T32</f>
         <v>4.4335746361316906</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="3">
         <f>SortedSpeaker!R33</f>
         <v>162.64024123092568</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <f>SortedSpeaker!S33</f>
         <v>21.376390611636417</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <f>SortedSpeaker!T33</f>
         <v>4.6384965726138301</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="3">
         <f>SortedSpeaker!R34</f>
         <v>-174.75770818188354</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <f>SortedSpeaker!S34</f>
         <v>13.332304509064471</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <f>SortedSpeaker!T34</f>
         <v>4.335242599906767</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="3">
         <f>SortedSpeaker!R35</f>
         <v>-174.75770818188354</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <f>SortedSpeaker!S35</f>
         <v>21.840490063843184</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
         <f>SortedSpeaker!T35</f>
         <v>4.5446006205217175</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="3">
         <f>SortedSpeaker!R36</f>
-        <v>24.47445674721007</v>
-      </c>
-      <c r="B35">
+        <v>-155.23479302123613</v>
+      </c>
+      <c r="B35" s="3">
         <f>SortedSpeaker!S36</f>
-        <v>34.601402800999509</v>
-      </c>
-      <c r="C35">
+        <v>34.572363524646619</v>
+      </c>
+      <c r="C35" s="3">
         <f>SortedSpeaker!T36</f>
-        <v>5.3921899420523145</v>
+        <v>5.3961549463881564</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="3">
         <f>SortedSpeaker!R37</f>
         <v>-152.82571739877736</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <f>SortedSpeaker!S37</f>
         <v>12.56703773496713</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3">
         <f>SortedSpeaker!T37</f>
         <v>4.5945946863127389</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="3">
         <f>SortedSpeaker!R38</f>
         <v>-152.82571739877736</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <f>SortedSpeaker!S38</f>
         <v>20.656854314257824</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3">
         <f>SortedSpeaker!T38</f>
         <v>4.7926367201670166</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="3">
         <f>SortedSpeaker!R39</f>
         <v>-133.7622102320463</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <f>SortedSpeaker!S39</f>
         <v>11.19050026689353</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3">
         <f>SortedSpeaker!T39</f>
         <v>5.1511888457907027</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="3">
         <f>SortedSpeaker!R40</f>
         <v>-133.7622102320463</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <f>SortedSpeaker!S40</f>
         <v>18.499039879728343</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <f>SortedSpeaker!T40</f>
         <v>5.3285845142024861</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="3">
         <f>SortedSpeaker!R41</f>
         <v>-117.98579358437399</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <f>SortedSpeaker!S41</f>
         <v>9.7417366465724218</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <f>SortedSpeaker!T41</f>
         <v>5.9081353505020484</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="3">
         <f>SortedSpeaker!R42</f>
         <v>-117.98579358437399</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <f>SortedSpeaker!S42</f>
         <v>16.19073271223106</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3">
         <f>SortedSpeaker!T42</f>
         <v>6.0634255763431248</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="3">
         <f>SortedSpeaker!R43</f>
-        <v>63.484236310055316</v>
-      </c>
-      <c r="B42">
+        <v>-116.3847475481442</v>
+      </c>
+      <c r="B42" s="3">
         <f>SortedSpeaker!S43</f>
-        <v>27.369461253572339</v>
-      </c>
-      <c r="C42">
+        <v>27.335757209509374</v>
+      </c>
+      <c r="C42" s="3">
         <f>SortedSpeaker!T43</f>
-        <v>6.6605469072204961</v>
+        <v>6.6681252151788772</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="3">
         <f>SortedSpeaker!R44</f>
         <v>-104.55545273114123</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="3">
         <f>SortedSpeaker!S44</f>
         <v>8.4445573083844039</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="3">
         <f>SortedSpeaker!T44</f>
         <v>6.8075195858220345</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="3">
         <f>SortedSpeaker!R45</f>
         <v>-104.55545273114123</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="3">
         <f>SortedSpeaker!S45</f>
         <v>14.094458060134764</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="3">
         <f>SortedSpeaker!T45</f>
         <v>6.9427220390384781</v>
       </c>
@@ -24468,7 +24611,7 @@
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <f>SortedSpeaker!R46</f>
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="B45" s="3">
         <f>SortedSpeaker!S46</f>
@@ -24500,637 +24643,637 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C45"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3">
+      <c r="A1" s="10">
         <f>SortedSpeaker!V2</f>
         <v>-69.366904439320834</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="10">
         <f>SortedSpeaker!W2</f>
         <v>-6.8004195298063834</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="10">
         <f>SortedSpeaker!X2</f>
         <v>6.3363917691767719</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="10">
         <f>SortedSpeaker!V3</f>
         <v>-69.366904439320834</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="10">
         <f>SortedSpeaker!W3</f>
         <v>-0.53999366131212634</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="10">
         <f>SortedSpeaker!X3</f>
         <v>6.292092422437161</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="10">
         <f>SortedSpeaker!V4</f>
         <v>-63.423065276213393</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="10">
         <f>SortedSpeaker!W4</f>
         <v>12.514751523165046</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="10">
         <f>SortedSpeaker!X4</f>
         <v>6.0548440070378629</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="10">
         <f>SortedSpeaker!V5</f>
         <v>-55.140915780735916</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="10">
         <f>SortedSpeaker!W5</f>
         <v>-7.8367439186346948</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="10">
         <f>SortedSpeaker!X5</f>
         <v>5.5027134122358774</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="10">
         <f>SortedSpeaker!V6</f>
         <v>-55.140915780735916</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="10">
         <f>SortedSpeaker!W6</f>
         <v>-0.62324443544919728</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="10">
         <f>SortedSpeaker!X6</f>
         <v>5.4516439077768659</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="10">
         <f>SortedSpeaker!V7</f>
         <v>-37.896354740302939</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="10">
         <f>SortedSpeaker!W7</f>
         <v>-8.9551418644697254</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="10">
         <f>SortedSpeaker!X7</f>
         <v>4.8200856585919185</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="10">
         <f>SortedSpeaker!V8</f>
         <v>-37.896354740302939</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="10">
         <f>SortedSpeaker!W8</f>
         <v>-0.71355338645747979</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="10">
         <f>SortedSpeaker!X8</f>
         <v>4.761700552970912</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="10">
         <f>SortedSpeaker!V9</f>
         <v>-25.233336704771727</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="10">
         <f>SortedSpeaker!W9</f>
         <v>16.440246799953421</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="10">
         <f>SortedSpeaker!X9</f>
         <v>4.6358986472437804</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="10">
         <f>SortedSpeaker!V10</f>
         <v>-17.359758769074336</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="10">
         <f>SortedSpeaker!W10</f>
         <v>-9.8542271259887713</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="10">
         <f>SortedSpeaker!X10</f>
         <v>4.3840773321361759</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="10">
         <f>SortedSpeaker!V11</f>
         <v>-17.359758769074336</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <f>SortedSpeaker!W11</f>
         <v>-0.78655119633682291</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="10">
         <f>SortedSpeaker!X11</f>
         <v>4.3198032888258062</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="10">
         <f>SortedSpeaker!V12</f>
         <v>5.2422918181164526</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="10">
         <f>SortedSpeaker!W12</f>
         <v>-10.085358760880604</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="10">
         <f>SortedSpeaker!X12</f>
         <v>4.2846094804598449</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="10">
         <f>SortedSpeaker!V13</f>
         <v>5.2422918181164526</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="10">
         <f>SortedSpeaker!W13</f>
         <v>-0.80537955314906851</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="10">
         <f>SortedSpeaker!X13</f>
         <v>4.2188203090492467</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="10">
         <f>SortedSpeaker!V14</f>
         <v>24.765206978763871</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="10">
         <f>SortedSpeaker!W14</f>
         <v>16.451142441190825</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="10">
         <f>SortedSpeaker!X14</f>
         <v>4.6329130366789064</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="10">
         <f>SortedSpeaker!V15</f>
         <v>27.174282601222639</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="10">
         <f>SortedSpeaker!W15</f>
         <v>-9.4981243640186612</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="10">
         <f>SortedSpeaker!X15</f>
         <v>4.5468505948066138</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="10">
         <f>SortedSpeaker!V16</f>
         <v>27.174282601222639</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="10">
         <f>SortedSpeaker!W16</f>
         <v>-0.75759353337381263</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="10">
         <f>SortedSpeaker!X16</f>
         <v>4.4849098911230376</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="10">
         <f>SortedSpeaker!V17</f>
         <v>46.237789767953686</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="10">
         <f>SortedSpeaker!W17</f>
         <v>-8.4454989406620768</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="10">
         <f>SortedSpeaker!X17</f>
         <v>5.1086491878967912</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17" s="10">
         <f>SortedSpeaker!V18</f>
         <v>46.237789767953686</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="10">
         <f>SortedSpeaker!W18</f>
         <v>-0.67233622934833437</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="10">
         <f>SortedSpeaker!X18</f>
         <v>5.0535990071431813</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="10">
         <f>SortedSpeaker!V19</f>
         <v>62.014206415626006</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="10">
         <f>SortedSpeaker!W19</f>
         <v>-7.3422412447084895</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="10">
         <f>SortedSpeaker!X19</f>
         <v>5.8710828064209721</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="A19" s="10">
         <f>SortedSpeaker!V20</f>
         <v>62.014206415626006</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="10">
         <f>SortedSpeaker!W20</f>
         <v>-0.58347168653298509</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="10">
         <f>SortedSpeaker!X20</f>
         <v>5.8232447758832846</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="A20" s="10">
         <f>SortedSpeaker!V21</f>
         <v>63.615252451855795</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="10">
         <f>SortedSpeaker!W21</f>
         <v>12.489133495552117</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="10">
         <f>SortedSpeaker!X21</f>
         <v>6.0670659206328352</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="A21" s="10">
         <f>SortedSpeaker!V22</f>
         <v>75.44454726885877</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="10">
         <f>SortedSpeaker!W22</f>
         <v>-6.3579207153954114</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="10">
         <f>SortedSpeaker!X22</f>
         <v>6.7753872886611139</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="A22" s="10">
         <f>SortedSpeaker!V23</f>
         <v>75.44454726885877</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="10">
         <f>SortedSpeaker!W23</f>
         <v>-0.50455828688097459</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="10">
         <f>SortedSpeaker!X23</f>
         <v>6.7339764858032147</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="A23" s="10">
         <f>SortedSpeaker!V24</f>
         <v>110.63309556067915</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="10">
         <f>SortedSpeaker!W24</f>
         <v>-6.8004195298063834</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="10">
         <f>SortedSpeaker!X24</f>
         <v>6.3363917691767719</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24" s="10">
         <f>SortedSpeaker!V25</f>
         <v>110.63309556067915</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="10">
         <f>SortedSpeaker!W25</f>
         <v>-0.53999366131212634</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="10">
         <f>SortedSpeaker!X25</f>
         <v>6.292092422437161</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="A25" s="10">
         <f>SortedSpeaker!V26</f>
-        <v>-63.398428921421988</v>
-      </c>
-      <c r="B25" s="3">
+        <v>116.57693472378661</v>
+      </c>
+      <c r="B25" s="10">
         <f>SortedSpeaker!W26</f>
-        <v>12.518021148079114</v>
-      </c>
-      <c r="C25" s="3">
+        <v>12.514751523165046</v>
+      </c>
+      <c r="C25" s="10">
         <f>SortedSpeaker!X26</f>
-        <v>6.0532877555740647</v>
+        <v>6.0548440070378629</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26" s="10">
         <f>SortedSpeaker!V27</f>
         <v>124.85908421926409</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="10">
         <f>SortedSpeaker!W27</f>
         <v>-7.8367439186346948</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="10">
         <f>SortedSpeaker!X27</f>
         <v>5.5027134122358774</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27" s="10">
         <f>SortedSpeaker!V28</f>
         <v>124.85908421926409</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="10">
         <f>SortedSpeaker!W28</f>
         <v>-0.62324443544919728</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="10">
         <f>SortedSpeaker!X28</f>
         <v>5.4516439077768659</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28" s="10">
         <f>SortedSpeaker!V29</f>
         <v>142.10364525969706</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="10">
         <f>SortedSpeaker!W29</f>
         <v>-8.9551418644697254</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="10">
         <f>SortedSpeaker!X29</f>
         <v>4.8200856585919185</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29" s="10">
         <f>SortedSpeaker!V30</f>
         <v>142.10364525969706</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="10">
         <f>SortedSpeaker!W30</f>
         <v>-0.71355338645747979</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="10">
         <f>SortedSpeaker!X30</f>
         <v>4.761700552970912</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30" s="10">
         <f>SortedSpeaker!V31</f>
-        <v>-24.503522137434636</v>
-      </c>
-      <c r="B30" s="3">
+        <v>154.76666329522828</v>
+      </c>
+      <c r="B30" s="10">
         <f>SortedSpeaker!W31</f>
-        <v>16.485382316912638</v>
-      </c>
-      <c r="C30" s="3">
+        <v>16.440246799953421</v>
+      </c>
+      <c r="C30" s="10">
         <f>SortedSpeaker!X31</f>
-        <v>4.6235567339399122</v>
+        <v>4.6358986472437804</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31" s="10">
         <f>SortedSpeaker!V32</f>
         <v>162.64024123092568</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="10">
         <f>SortedSpeaker!W32</f>
         <v>-9.8542271259887713</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="10">
         <f>SortedSpeaker!X32</f>
         <v>4.3840773321361759</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="A32" s="10">
         <f>SortedSpeaker!V33</f>
         <v>162.64024123092568</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="10">
         <f>SortedSpeaker!W33</f>
         <v>-0.78655119633682291</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="10">
         <f>SortedSpeaker!X33</f>
         <v>4.3198032888258062</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="A33" s="10">
         <f>SortedSpeaker!V34</f>
         <v>-174.75770818188354</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="10">
         <f>SortedSpeaker!W34</f>
         <v>-10.085358760880604</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="10">
         <f>SortedSpeaker!X34</f>
         <v>4.2846094804598449</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34" s="10">
         <f>SortedSpeaker!V35</f>
         <v>-174.75770818188354</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="10">
         <f>SortedSpeaker!W35</f>
         <v>-0.80537955314906851</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="10">
         <f>SortedSpeaker!X35</f>
         <v>4.2188203090492467</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="A35" s="10">
         <f>SortedSpeaker!V36</f>
-        <v>24.47445674721007</v>
-      </c>
-      <c r="B35" s="3">
+        <v>-155.23479302123613</v>
+      </c>
+      <c r="B35" s="10">
         <f>SortedSpeaker!W36</f>
-        <v>16.468027189366833</v>
-      </c>
-      <c r="C35" s="3">
+        <v>16.451142441190825</v>
+      </c>
+      <c r="C35" s="10">
         <f>SortedSpeaker!X36</f>
-        <v>4.628294218302262</v>
+        <v>4.6329130366789064</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="A36" s="10">
         <f>SortedSpeaker!V37</f>
         <v>-152.82571739877736</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="10">
         <f>SortedSpeaker!W37</f>
         <v>-9.4981243640186612</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="10">
         <f>SortedSpeaker!X37</f>
         <v>4.5468505948066138</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="A37" s="10">
         <f>SortedSpeaker!V38</f>
         <v>-152.82571739877736</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="10">
         <f>SortedSpeaker!W38</f>
         <v>-0.75759353337381263</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="10">
         <f>SortedSpeaker!X38</f>
         <v>4.4849098911230376</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="A38" s="10">
         <f>SortedSpeaker!V39</f>
         <v>-133.7622102320463</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="10">
         <f>SortedSpeaker!W39</f>
         <v>-8.4454989406620768</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="10">
         <f>SortedSpeaker!X39</f>
         <v>5.1086491878967912</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+      <c r="A39" s="10">
         <f>SortedSpeaker!V40</f>
         <v>-133.7622102320463</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="10">
         <f>SortedSpeaker!W40</f>
         <v>-0.67233622934833437</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="10">
         <f>SortedSpeaker!X40</f>
         <v>5.0535990071431813</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+      <c r="A40" s="10">
         <f>SortedSpeaker!V41</f>
         <v>-117.98579358437399</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="10">
         <f>SortedSpeaker!W41</f>
         <v>-7.3422412447084895</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="10">
         <f>SortedSpeaker!X41</f>
         <v>5.8710828064209721</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+      <c r="A41" s="10">
         <f>SortedSpeaker!V42</f>
         <v>-117.98579358437399</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="10">
         <f>SortedSpeaker!W42</f>
         <v>-0.58347168653298509</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="10">
         <f>SortedSpeaker!X42</f>
         <v>5.8232447758832846</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+      <c r="A42" s="10">
         <f>SortedSpeaker!V43</f>
-        <v>63.484236310055316</v>
-      </c>
-      <c r="B42" s="3">
+        <v>-116.3847475481442</v>
+      </c>
+      <c r="B42" s="10">
         <f>SortedSpeaker!W43</f>
-        <v>12.506582442617592</v>
-      </c>
-      <c r="C42" s="3">
+        <v>12.489133495552117</v>
+      </c>
+      <c r="C42" s="10">
         <f>SortedSpeaker!X43</f>
-        <v>6.0587358502648483</v>
+        <v>6.0670659206328352</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43" s="10">
         <f>SortedSpeaker!V44</f>
         <v>-104.55545273114123</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="10">
         <f>SortedSpeaker!W44</f>
         <v>-6.3579207153954114</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="10">
         <f>SortedSpeaker!X44</f>
         <v>6.7753872886611139</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+      <c r="A44" s="10">
         <f>SortedSpeaker!V45</f>
         <v>-104.55545273114123</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="10">
         <f>SortedSpeaker!W45</f>
         <v>-0.50455828688097459</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="10">
         <f>SortedSpeaker!X45</f>
         <v>6.7339764858032147</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+      <c r="A45" s="10">
         <f>SortedSpeaker!V46</f>
-        <v>0</v>
-      </c>
-      <c r="B45" s="3">
+        <v>-90</v>
+      </c>
+      <c r="B45" s="10">
         <f>SortedSpeaker!W46</f>
         <v>81.538783529194319</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="10">
         <f>SortedSpeaker!X46</f>
         <v>2.0388757578273378</v>
       </c>
@@ -25144,638 +25287,638 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76C94A7-CFDF-184F-AB55-C23BA4B86F04}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C45"/>
+    <sheetView topLeftCell="A4" zoomScale="102" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3">
+      <c r="A1" s="10">
         <f>SortedSpeaker!Z2</f>
         <v>-69.366904439320834</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="10">
         <f>SortedSpeaker!AA2</f>
         <v>-9.1551706518664009</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="10">
         <f>SortedSpeaker!AB2</f>
         <v>6.3729982396428717</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="10">
         <f>SortedSpeaker!Z3</f>
         <v>-69.366904439320834</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="10">
         <f>SortedSpeaker!AA3</f>
         <v>-2.9387880520458696</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="10">
         <f>SortedSpeaker!AB3</f>
         <v>6.3000983772073864</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="10">
         <f>SortedSpeaker!Z4</f>
         <v>-63.423065276213393</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="10">
         <f>SortedSpeaker!AA4</f>
         <v>10.056999542825952</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="10">
         <f>SortedSpeaker!AB4</f>
         <v>6.0032248848066923</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="10">
         <f>SortedSpeaker!Z5</f>
         <v>-55.140915780735916</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="10">
         <f>SortedSpeaker!AA5</f>
         <v>-10.537158792071354</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="10">
         <f>SortedSpeaker!AB5</f>
         <v>5.5448264902700624</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="10">
         <f>SortedSpeaker!Z6</f>
         <v>-55.140915780735916</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="10">
         <f>SortedSpeaker!AA6</f>
         <v>-3.3909072024217428</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="10">
         <f>SortedSpeaker!AB6</f>
         <v>5.4608821455146437</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="10">
         <f>SortedSpeaker!Z7</f>
         <v>-37.896354740302939</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="10">
         <f>SortedSpeaker!AA7</f>
         <v>-12.02242380905775</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="10">
         <f>SortedSpeaker!AB7</f>
         <v>4.8681076062638029</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="10">
         <f>SortedSpeaker!Z8</f>
         <v>-37.896354740302939</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="10">
         <f>SortedSpeaker!AA8</f>
         <v>-3.8808947854382496</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="10">
         <f>SortedSpeaker!AB8</f>
         <v>4.7722745799213495</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="10">
         <f>SortedSpeaker!Z9</f>
         <v>-25.233336704771727</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="10">
         <f>SortedSpeaker!AA9</f>
         <v>13.26649045905646</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="10">
         <f>SortedSpeaker!AB9</f>
         <v>4.5682742185114842</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="10">
         <f>SortedSpeaker!Z10</f>
         <v>-17.359758769074336</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="10">
         <f>SortedSpeaker!AA10</f>
         <v>-13.211249325077995</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="10">
         <f>SortedSpeaker!AB10</f>
         <v>4.4368209299170784</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="10">
         <f>SortedSpeaker!Z11</f>
         <v>-17.359758769074336</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <f>SortedSpeaker!AA11</f>
         <v>-4.2765598380915124</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="10">
         <f>SortedSpeaker!AB11</f>
         <v>4.3314562175035602</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="10">
         <f>SortedSpeaker!Z12</f>
         <v>5.2422918181164526</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="10">
         <f>SortedSpeaker!AA12</f>
         <v>-13.516063363591293</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="10">
         <f>SortedSpeaker!AB12</f>
         <v>4.3385624704556669</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="10">
         <f>SortedSpeaker!Z13</f>
         <v>5.2422918181164526</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="10">
         <f>SortedSpeaker!AA13</f>
         <v>-4.3785513511579257</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="10">
         <f>SortedSpeaker!AB13</f>
         <v>4.2307513883524734</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="10">
         <f>SortedSpeaker!Z14</f>
         <v>24.765206978763871</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="10">
         <f>SortedSpeaker!AA14</f>
         <v>13.275456050147248</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="10">
         <f>SortedSpeaker!AB14</f>
         <v>4.5652443826622653</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="10">
         <f>SortedSpeaker!Z15</f>
         <v>27.174282601222639</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="10">
         <f>SortedSpeaker!AA15</f>
         <v>-12.740971812728684</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="10">
         <f>SortedSpeaker!AB15</f>
         <v>4.5977272909007176</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="10">
         <f>SortedSpeaker!Z16</f>
         <v>27.174282601222639</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="10">
         <f>SortedSpeaker!AA16</f>
         <v>-4.1196477900941169</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="10">
         <f>SortedSpeaker!AB16</f>
         <v>4.496134922518813</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="10">
         <f>SortedSpeaker!Z17</f>
         <v>46.237789767953686</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="10">
         <f>SortedSpeaker!AA17</f>
         <v>-11.346448197505596</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="10">
         <f>SortedSpeaker!AB17</f>
         <v>5.1539831620794558</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17" s="10">
         <f>SortedSpeaker!Z18</f>
         <v>46.237789767953686</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="10">
         <f>SortedSpeaker!AA18</f>
         <v>-3.6573275784143031</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="10">
         <f>SortedSpeaker!AB18</f>
         <v>5.063563511500428</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="10">
         <f>SortedSpeaker!Z19</f>
         <v>62.014206415626006</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="10">
         <f>SortedSpeaker!AA19</f>
         <v>-9.8783589719401519</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="10">
         <f>SortedSpeaker!AB19</f>
         <v>5.9105718191941428</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="A19" s="10">
         <f>SortedSpeaker!Z20</f>
         <v>62.014206415626006</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="10">
         <f>SortedSpeaker!AA20</f>
         <v>-3.1749565589924145</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="10">
         <f>SortedSpeaker!AB20</f>
         <v>5.8318943946072928</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="A20" s="10">
         <f>SortedSpeaker!Z21</f>
         <v>63.615252451855795</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="10">
         <f>SortedSpeaker!AA21</f>
         <v>10.036177586498006</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="10">
         <f>SortedSpeaker!AB21</f>
         <v>6.0155516748926976</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="A21" s="10">
         <f>SortedSpeaker!Z22</f>
         <v>75.44454726885877</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="10">
         <f>SortedSpeaker!AA22</f>
         <v>-8.5635721303178229</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="10">
         <f>SortedSpeaker!AB22</f>
         <v>6.809634264874334</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="A22" s="10">
         <f>SortedSpeaker!Z23</f>
         <v>75.44454726885877</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="10">
         <f>SortedSpeaker!AA23</f>
         <v>-2.7462346530811899</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="10">
         <f>SortedSpeaker!AB23</f>
         <v>6.7414576926174208</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="A23" s="10">
         <f>SortedSpeaker!Z24</f>
         <v>110.63309556067915</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="10">
         <f>SortedSpeaker!AA24</f>
         <v>-9.1551706518664009</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="10">
         <f>SortedSpeaker!AB24</f>
         <v>6.3729982396428717</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24" s="10">
         <f>SortedSpeaker!Z25</f>
         <v>110.63309556067915</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="10">
         <f>SortedSpeaker!AA25</f>
         <v>-2.9387880520458696</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="10">
         <f>SortedSpeaker!AB25</f>
         <v>6.3000983772073864</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="A25" s="10">
         <f>SortedSpeaker!Z26</f>
-        <v>-63.398428921421988</v>
-      </c>
-      <c r="B25" s="3">
+        <v>116.57693472378661</v>
+      </c>
+      <c r="B25" s="10">
         <f>SortedSpeaker!AA26</f>
-        <v>10.059657150098166</v>
-      </c>
-      <c r="C25" s="3">
+        <v>10.056999542825952</v>
+      </c>
+      <c r="C25" s="10">
         <f>SortedSpeaker!AB26</f>
-        <v>6.0016552483279897</v>
+        <v>6.0032248848066923</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26" s="10">
         <f>SortedSpeaker!Z27</f>
         <v>124.85908421926409</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="10">
         <f>SortedSpeaker!AA27</f>
         <v>-10.537158792071354</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="10">
         <f>SortedSpeaker!AB27</f>
         <v>5.5448264902700624</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27" s="10">
         <f>SortedSpeaker!Z28</f>
         <v>124.85908421926409</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="10">
         <f>SortedSpeaker!AA28</f>
         <v>-3.3909072024217428</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="10">
         <f>SortedSpeaker!AB28</f>
         <v>5.4608821455146437</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28" s="10">
         <f>SortedSpeaker!Z29</f>
         <v>142.10364525969706</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="10">
         <f>SortedSpeaker!AA29</f>
         <v>-12.02242380905775</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="10">
         <f>SortedSpeaker!AB29</f>
         <v>4.8681076062638029</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29" s="10">
         <f>SortedSpeaker!Z30</f>
         <v>142.10364525969706</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="10">
         <f>SortedSpeaker!AA30</f>
         <v>-3.8808947854382496</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="10">
         <f>SortedSpeaker!AB30</f>
         <v>4.7722745799213495</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30" s="10">
         <f>SortedSpeaker!Z31</f>
-        <v>-24.503522137434636</v>
-      </c>
-      <c r="B30" s="3">
+        <v>154.76666329522828</v>
+      </c>
+      <c r="B30" s="10">
         <f>SortedSpeaker!AA31</f>
-        <v>13.303632931919649</v>
-      </c>
-      <c r="C30" s="3">
+        <v>13.26649045905646</v>
+      </c>
+      <c r="C30" s="10">
         <f>SortedSpeaker!AB31</f>
-        <v>4.5557491085397919</v>
+        <v>4.5682742185114842</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31" s="10">
         <f>SortedSpeaker!Z32</f>
         <v>162.64024123092568</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="10">
         <f>SortedSpeaker!AA32</f>
         <v>-13.211249325077995</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="10">
         <f>SortedSpeaker!AB32</f>
         <v>4.4368209299170784</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="A32" s="10">
         <f>SortedSpeaker!Z33</f>
         <v>162.64024123092568</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="10">
         <f>SortedSpeaker!AA33</f>
         <v>-4.2765598380915124</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="10">
         <f>SortedSpeaker!AB33</f>
         <v>4.3314562175035602</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="A33" s="10">
         <f>SortedSpeaker!Z34</f>
         <v>-174.75770818188354</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="10">
         <f>SortedSpeaker!AA34</f>
         <v>-13.516063363591293</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="10">
         <f>SortedSpeaker!AB34</f>
         <v>4.3385624704556669</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34" s="10">
         <f>SortedSpeaker!Z35</f>
         <v>-174.75770818188354</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="10">
         <f>SortedSpeaker!AA35</f>
         <v>-4.3785513511579257</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="10">
         <f>SortedSpeaker!AB35</f>
         <v>4.2307513883524734</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="A35" s="10">
         <f>SortedSpeaker!Z36</f>
-        <v>24.47445674721007</v>
-      </c>
-      <c r="B35" s="3">
+        <v>-155.23479302123613</v>
+      </c>
+      <c r="B35" s="10">
         <f>SortedSpeaker!AA36</f>
-        <v>13.289350521250501</v>
-      </c>
-      <c r="C35" s="3">
+        <v>13.275456050147248</v>
+      </c>
+      <c r="C35" s="10">
         <f>SortedSpeaker!AB36</f>
-        <v>4.5605570316760806</v>
+        <v>4.5652443826622653</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="A36" s="10">
         <f>SortedSpeaker!Z37</f>
         <v>-152.82571739877736</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="10">
         <f>SortedSpeaker!AA37</f>
         <v>-12.740971812728684</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="10">
         <f>SortedSpeaker!AB37</f>
         <v>4.5977272909007176</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="A37" s="10">
         <f>SortedSpeaker!Z38</f>
         <v>-152.82571739877736</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="10">
         <f>SortedSpeaker!AA38</f>
         <v>-4.1196477900941169</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="10">
         <f>SortedSpeaker!AB38</f>
         <v>4.496134922518813</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="A38" s="10">
         <f>SortedSpeaker!Z39</f>
         <v>-133.7622102320463</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="10">
         <f>SortedSpeaker!AA39</f>
         <v>-11.346448197505596</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="10">
         <f>SortedSpeaker!AB39</f>
         <v>5.1539831620794558</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+      <c r="A39" s="10">
         <f>SortedSpeaker!Z40</f>
         <v>-133.7622102320463</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="10">
         <f>SortedSpeaker!AA40</f>
         <v>-3.6573275784143031</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="10">
         <f>SortedSpeaker!AB40</f>
         <v>5.063563511500428</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+      <c r="A40" s="10">
         <f>SortedSpeaker!Z41</f>
         <v>-117.98579358437399</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="10">
         <f>SortedSpeaker!AA41</f>
         <v>-9.8783589719401519</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="10">
         <f>SortedSpeaker!AB41</f>
         <v>5.9105718191941428</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+      <c r="A41" s="10">
         <f>SortedSpeaker!Z42</f>
         <v>-117.98579358437399</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="10">
         <f>SortedSpeaker!AA42</f>
         <v>-3.1749565589924145</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="10">
         <f>SortedSpeaker!AB42</f>
         <v>5.8318943946072928</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+      <c r="A42" s="10">
         <f>SortedSpeaker!Z43</f>
-        <v>63.484236310055316</v>
-      </c>
-      <c r="B42" s="3">
+        <v>-116.3847475481442</v>
+      </c>
+      <c r="B42" s="10">
         <f>SortedSpeaker!AA43</f>
-        <v>10.050359677020113</v>
-      </c>
-      <c r="C42" s="3">
+        <v>10.036177586498006</v>
+      </c>
+      <c r="C42" s="10">
         <f>SortedSpeaker!AB43</f>
-        <v>6.0071501705288268</v>
+        <v>6.0155516748926976</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43" s="10">
         <f>SortedSpeaker!Z44</f>
         <v>-104.55545273114123</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="10">
         <f>SortedSpeaker!AA44</f>
         <v>-8.5635721303178229</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="10">
         <f>SortedSpeaker!AB44</f>
         <v>6.809634264874334</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+      <c r="A44" s="10">
         <f>SortedSpeaker!Z45</f>
         <v>-104.55545273114123</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="10">
         <f>SortedSpeaker!AA45</f>
         <v>-2.7462346530811899</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="10">
         <f>SortedSpeaker!AB45</f>
         <v>6.7414576926174208</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+      <c r="A45" s="10">
         <f>SortedSpeaker!Z46</f>
-        <v>0</v>
-      </c>
-      <c r="B45" s="3">
+        <v>-90</v>
+      </c>
+      <c r="B45" s="10">
         <f>SortedSpeaker!AA46</f>
         <v>80.28866454423698</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="10">
         <f>SortedSpeaker!AB46</f>
         <v>1.7784692587323516</v>
       </c>
@@ -25789,8 +25932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EFE4AA-4C89-C04B-B3EB-82F915980C24}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C45"/>
+    <sheetView zoomScale="104" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26138,11 +26281,11 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <f>SortedSpeaker!F26</f>
-        <v>-5.2838320181506457</v>
+        <v>5.2863950181506461</v>
       </c>
       <c r="B25" s="10">
         <f>SortedSpeaker!G26</f>
-        <v>2.6461271955159247</v>
+        <v>-2.6445681955159244</v>
       </c>
       <c r="C25" s="10">
         <f>SortedSpeaker!H26</f>
@@ -26208,11 +26351,11 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <f>SortedSpeaker!F31</f>
-        <v>-1.8387873034655597</v>
+        <v>1.8955093034655597</v>
       </c>
       <c r="B30" s="10">
         <f>SortedSpeaker!G31</f>
-        <v>4.0341932779274421</v>
+        <v>-4.0220862779274418</v>
       </c>
       <c r="C30" s="10">
         <f>SortedSpeaker!H31</f>
@@ -26278,11 +26421,11 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
         <f>SortedSpeaker!F36</f>
-        <v>1.8387873034655597</v>
+        <v>-1.8612803034655598</v>
       </c>
       <c r="B35" s="10">
         <f>SortedSpeaker!G36</f>
-        <v>4.0396219999999996</v>
+        <v>-4.034612263459838</v>
       </c>
       <c r="C35" s="10">
         <f>SortedSpeaker!H36</f>
@@ -26376,11 +26519,11 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
         <f>SortedSpeaker!F43</f>
-        <v>5.2927826070532085</v>
+        <v>-5.3064506070532076</v>
       </c>
       <c r="B42" s="10">
         <f>SortedSpeaker!G43</f>
-        <v>2.6407024930611844</v>
+        <v>-2.6323844930611839</v>
       </c>
       <c r="C42" s="10">
         <f>SortedSpeaker!H43</f>
@@ -26456,631 +26599,631 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="10">
+      <c r="A1" s="3">
         <f>SortedSpeaker!J2</f>
         <v>-5.8882318492012526</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="3">
         <f>SortedSpeaker!K2</f>
         <v>2.2171234184282875</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="3">
         <f>SortedSpeaker!L2</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+      <c r="A2" s="3">
         <f>SortedSpeaker!J3</f>
         <v>-5.8882318492012526</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="3">
         <f>SortedSpeaker!K3</f>
         <v>2.2171234184282875</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="3">
         <f>SortedSpeaker!L3</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="A3" s="3">
         <f>SortedSpeaker!J4</f>
         <v>-5.2863950181506461</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="3">
         <f>SortedSpeaker!K4</f>
         <v>2.6445681955159244</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="3">
         <f>SortedSpeaker!L4</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="A4" s="3">
         <f>SortedSpeaker!J5</f>
         <v>-4.4731376070532081</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="3">
         <f>SortedSpeaker!K5</f>
         <v>3.1157574930611842</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="3">
         <f>SortedSpeaker!L5</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="A5" s="3">
         <f>SortedSpeaker!J6</f>
         <v>-4.4731376070532081</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="3">
         <f>SortedSpeaker!K6</f>
         <v>3.1157574930611842</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="3">
         <f>SortedSpeaker!L6</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+      <c r="A6" s="3">
         <f>SortedSpeaker!J7</f>
         <v>-2.9245763063212125</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="3">
         <f>SortedSpeaker!K7</f>
         <v>3.7572768190097552</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="3">
         <f>SortedSpeaker!L7</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
+      <c r="A7" s="3">
         <f>SortedSpeaker!J8</f>
         <v>-2.9245763063212125</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="3">
         <f>SortedSpeaker!K8</f>
         <v>3.7572768190097552</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="3">
         <f>SortedSpeaker!L8</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+      <c r="A8" s="3">
         <f>SortedSpeaker!J9</f>
         <v>-1.8955093034655597</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="3">
         <f>SortedSpeaker!K9</f>
         <v>4.0220862779274418</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="3">
         <f>SortedSpeaker!L9</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="A9" s="3">
         <f>SortedSpeaker!J10</f>
         <v>-1.2887804858284249</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="3">
         <f>SortedSpeaker!K10</f>
         <v>4.1226482779274418</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="3">
         <f>SortedSpeaker!L10</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="3">
         <f>SortedSpeaker!J11</f>
         <v>-1.2887804858284249</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="3">
         <f>SortedSpeaker!K11</f>
         <v>4.1226482779274418</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="3">
         <f>SortedSpeaker!L11</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+      <c r="A11" s="3">
         <f>SortedSpeaker!J12</f>
         <v>0.38542561297257855</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="3">
         <f>SortedSpeaker!K12</f>
         <v>4.2007589084486971</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="3">
         <f>SortedSpeaker!L12</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+      <c r="A12" s="3">
         <f>SortedSpeaker!J13</f>
         <v>0.38542561297257855</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="3">
         <f>SortedSpeaker!K13</f>
         <v>4.2007589084486971</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="3">
         <f>SortedSpeaker!L13</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="10">
+      <c r="A13" s="3">
         <f>SortedSpeaker!J14</f>
         <v>1.8612803034655598</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="3">
         <f>SortedSpeaker!K14</f>
         <v>4.034612263459838</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="3">
         <f>SortedSpeaker!L14</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
+      <c r="A14" s="3">
         <f>SortedSpeaker!J15</f>
         <v>2.0480733034655594</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="3">
         <f>SortedSpeaker!K15</f>
         <v>3.9895232779274425</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="3">
         <f>SortedSpeaker!L15</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+      <c r="A15" s="3">
         <f>SortedSpeaker!J16</f>
         <v>2.0480733034655594</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="3">
         <f>SortedSpeaker!K16</f>
         <v>3.9895232779274425</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="3">
         <f>SortedSpeaker!L16</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
+      <c r="A16" s="3">
         <f>SortedSpeaker!J17</f>
         <v>3.6495417006109956</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="3">
         <f>SortedSpeaker!K17</f>
         <v>3.4951669216934333</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="3">
         <f>SortedSpeaker!L17</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
+      <c r="A17" s="3">
         <f>SortedSpeaker!J18</f>
         <v>3.6495417006109956</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="3">
         <f>SortedSpeaker!K18</f>
         <v>3.4951669216934333</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="3">
         <f>SortedSpeaker!L18</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
+      <c r="A18" s="3">
         <f>SortedSpeaker!J19</f>
         <v>5.1420310181506466</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="3">
         <f>SortedSpeaker!K19</f>
         <v>2.7324311955159244</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="3">
         <f>SortedSpeaker!L19</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
+      <c r="A19" s="3">
         <f>SortedSpeaker!J20</f>
         <v>5.1420310181506466</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="3">
         <f>SortedSpeaker!K20</f>
         <v>2.7324311955159244</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="3">
         <f>SortedSpeaker!L20</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
+      <c r="A20" s="3">
         <f>SortedSpeaker!J21</f>
         <v>5.3064506070532076</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="3">
         <f>SortedSpeaker!K21</f>
         <v>2.6323844930611839</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="3">
         <f>SortedSpeaker!L21</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
+      <c r="A21" s="3">
         <f>SortedSpeaker!J22</f>
         <v>6.5175958492012525</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="3">
         <f>SortedSpeaker!K22</f>
         <v>1.6922964184282874</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="3">
         <f>SortedSpeaker!L22</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10">
+      <c r="A22" s="3">
         <f>SortedSpeaker!J23</f>
         <v>6.5175958492012525</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="3">
         <f>SortedSpeaker!K23</f>
         <v>1.6922964184282874</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="3">
         <f>SortedSpeaker!L23</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10">
+      <c r="A23" s="3">
         <f>SortedSpeaker!J24</f>
         <v>5.8882318492012526</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="3">
         <f>SortedSpeaker!K24</f>
         <v>-2.2171234184282875</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="3">
         <f>SortedSpeaker!L24</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="10">
+      <c r="A24" s="3">
         <f>SortedSpeaker!J25</f>
         <v>5.8882318492012526</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="3">
         <f>SortedSpeaker!K25</f>
         <v>-2.2171234184282875</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="3">
         <f>SortedSpeaker!L25</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
+      <c r="A25" s="3">
         <f>SortedSpeaker!J26</f>
-        <v>-5.2838320181506457</v>
-      </c>
-      <c r="B25" s="10">
+        <v>5.2863950181506461</v>
+      </c>
+      <c r="B25" s="3">
         <f>SortedSpeaker!K26</f>
-        <v>2.6461271955159247</v>
-      </c>
-      <c r="C25" s="10">
+        <v>-2.6445681955159244</v>
+      </c>
+      <c r="C25" s="3">
         <f>SortedSpeaker!L26</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
+      <c r="A26" s="3">
         <f>SortedSpeaker!J27</f>
         <v>4.4731376070532081</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="3">
         <f>SortedSpeaker!K27</f>
         <v>-3.1157574930611842</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="3">
         <f>SortedSpeaker!L27</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="10">
+      <c r="A27" s="3">
         <f>SortedSpeaker!J28</f>
         <v>4.4731376070532081</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="3">
         <f>SortedSpeaker!K28</f>
         <v>-3.1157574930611842</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="3">
         <f>SortedSpeaker!L28</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
+      <c r="A28" s="3">
         <f>SortedSpeaker!J29</f>
         <v>2.9245763063212125</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="3">
         <f>SortedSpeaker!K29</f>
         <v>-3.7572768190097552</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="3">
         <f>SortedSpeaker!L29</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
+      <c r="A29" s="3">
         <f>SortedSpeaker!J30</f>
         <v>2.9245763063212125</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="3">
         <f>SortedSpeaker!K30</f>
         <v>-3.7572768190097552</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="3">
         <f>SortedSpeaker!L30</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
+      <c r="A30" s="3">
         <f>SortedSpeaker!J31</f>
-        <v>-1.8387873034655597</v>
-      </c>
-      <c r="B30" s="10">
+        <v>1.8955093034655597</v>
+      </c>
+      <c r="B30" s="3">
         <f>SortedSpeaker!K31</f>
-        <v>4.0341932779274421</v>
-      </c>
-      <c r="C30" s="10">
+        <v>-4.0220862779274418</v>
+      </c>
+      <c r="C30" s="3">
         <f>SortedSpeaker!L31</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="10">
+      <c r="A31" s="3">
         <f>SortedSpeaker!J32</f>
         <v>1.2887804858284249</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="3">
         <f>SortedSpeaker!K32</f>
         <v>-4.1226482779274418</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="3">
         <f>SortedSpeaker!L32</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="10">
+      <c r="A32" s="3">
         <f>SortedSpeaker!J33</f>
         <v>1.2887804858284249</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="3">
         <f>SortedSpeaker!K33</f>
         <v>-4.1226482779274418</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="3">
         <f>SortedSpeaker!L33</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="10">
+      <c r="A33" s="3">
         <f>SortedSpeaker!J34</f>
         <v>-0.38542561297257855</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="3">
         <f>SortedSpeaker!K34</f>
         <v>-4.2007589084486971</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="3">
         <f>SortedSpeaker!L34</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="10">
+      <c r="A34" s="3">
         <f>SortedSpeaker!J35</f>
         <v>-0.38542561297257855</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="3">
         <f>SortedSpeaker!K35</f>
         <v>-4.2007589084486971</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="3">
         <f>SortedSpeaker!L35</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="10">
+      <c r="A35" s="3">
         <f>SortedSpeaker!J36</f>
-        <v>1.8387873034655597</v>
-      </c>
-      <c r="B35" s="10">
+        <v>-1.8612803034655598</v>
+      </c>
+      <c r="B35" s="3">
         <f>SortedSpeaker!K36</f>
-        <v>4.0396219999999996</v>
-      </c>
-      <c r="C35" s="10">
+        <v>-4.034612263459838</v>
+      </c>
+      <c r="C35" s="3">
         <f>SortedSpeaker!L36</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="10">
+      <c r="A36" s="3">
         <f>SortedSpeaker!J37</f>
         <v>-2.0480733034655594</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="3">
         <f>SortedSpeaker!K37</f>
         <v>-3.9895232779274425</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="3">
         <f>SortedSpeaker!L37</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="10">
+      <c r="A37" s="3">
         <f>SortedSpeaker!J38</f>
         <v>-2.0480733034655594</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="3">
         <f>SortedSpeaker!K38</f>
         <v>-3.9895232779274425</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="3">
         <f>SortedSpeaker!L38</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="10">
+      <c r="A38" s="3">
         <f>SortedSpeaker!J39</f>
         <v>-3.6495417006109956</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="3">
         <f>SortedSpeaker!K39</f>
         <v>-3.4951669216934333</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="3">
         <f>SortedSpeaker!L39</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="10">
+      <c r="A39" s="3">
         <f>SortedSpeaker!J40</f>
         <v>-3.6495417006109956</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="3">
         <f>SortedSpeaker!K40</f>
         <v>-3.4951669216934333</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="3">
         <f>SortedSpeaker!L40</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="10">
+      <c r="A40" s="3">
         <f>SortedSpeaker!J41</f>
         <v>-5.1420310181506466</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="3">
         <f>SortedSpeaker!K41</f>
         <v>-2.7324311955159244</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="3">
         <f>SortedSpeaker!L41</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="10">
+      <c r="A41" s="3">
         <f>SortedSpeaker!J42</f>
         <v>-5.1420310181506466</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="3">
         <f>SortedSpeaker!K42</f>
         <v>-2.7324311955159244</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="3">
         <f>SortedSpeaker!L42</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="10">
+      <c r="A42" s="3">
         <f>SortedSpeaker!J43</f>
-        <v>5.2927826070532085</v>
-      </c>
-      <c r="B42" s="10">
+        <v>-5.3064506070532076</v>
+      </c>
+      <c r="B42" s="3">
         <f>SortedSpeaker!K43</f>
-        <v>2.6407024930611844</v>
-      </c>
-      <c r="C42" s="10">
+        <v>-2.6323844930611839</v>
+      </c>
+      <c r="C42" s="3">
         <f>SortedSpeaker!L43</f>
         <v>1.31203</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="10">
+      <c r="A43" s="3">
         <f>SortedSpeaker!J44</f>
         <v>-6.5175958492012525</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="3">
         <f>SortedSpeaker!K44</f>
         <v>-1.6922964184282874</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="3">
         <f>SortedSpeaker!L44</f>
         <v>-0.75029999999999997</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="10">
+      <c r="A44" s="3">
         <f>SortedSpeaker!J45</f>
         <v>-6.5175958492012525</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="3">
         <f>SortedSpeaker!K45</f>
         <v>-1.6922964184282874</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="3">
         <f>SortedSpeaker!L45</f>
         <v>-5.9299999999999908E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="10">
+      <c r="A45" s="3">
         <f>SortedSpeaker!J46</f>
         <v>-0.3</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="3">
         <f>SortedSpeaker!K46</f>
         <v>0</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="3">
         <f>SortedSpeaker!L46</f>
         <v>2.0166840000000001</v>
       </c>
@@ -27106,7 +27249,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection sqref="A1:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27450,11 +27593,11 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <f>SortedSpeaker!N26</f>
-        <v>-5.2838320181506457</v>
+        <v>5.2863950181506461</v>
       </c>
       <c r="B25" s="10">
         <f>SortedSpeaker!O26</f>
-        <v>2.6461271955159247</v>
+        <v>-2.6445681955159244</v>
       </c>
       <c r="C25" s="10">
         <f>SortedSpeaker!P26</f>
@@ -27520,11 +27663,11 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <f>SortedSpeaker!N31</f>
-        <v>-1.8387873034655597</v>
+        <v>1.8955093034655597</v>
       </c>
       <c r="B30" s="10">
         <f>SortedSpeaker!O31</f>
-        <v>4.0341932779274421</v>
+        <v>-4.0220862779274418</v>
       </c>
       <c r="C30" s="10">
         <f>SortedSpeaker!P31</f>
@@ -27590,11 +27733,11 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
         <f>SortedSpeaker!N36</f>
-        <v>1.8387873034655597</v>
+        <v>-1.8612803034655598</v>
       </c>
       <c r="B35" s="10">
         <f>SortedSpeaker!O36</f>
-        <v>4.0396219999999996</v>
+        <v>-4.034612263459838</v>
       </c>
       <c r="C35" s="10">
         <f>SortedSpeaker!P36</f>
@@ -27688,11 +27831,11 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
         <f>SortedSpeaker!N43</f>
-        <v>5.2927826070532085</v>
+        <v>-5.3064506070532076</v>
       </c>
       <c r="B42" s="10">
         <f>SortedSpeaker!O43</f>
-        <v>2.6407024930611844</v>
+        <v>-2.6323844930611839</v>
       </c>
       <c r="C42" s="10">
         <f>SortedSpeaker!P43</f>

</xml_diff>